<commit_message>
chore: update score 2 persons
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/node/dflyapp/tennis-btn/pages/api/score/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9D2548-93B4-044C-9EEE-800413EA0CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060B407A-5066-1C42-9DE5-C773C96DAA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3300" yWindow="760" windowWidth="27860" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5924,8 +5924,8 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A713" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F759" sqref="F759"/>
+      <pane ySplit="4" topLeftCell="A732" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E756" sqref="E756"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -38644,32 +38644,18 @@
       </c>
       <c r="B706" s="1"/>
       <c r="C706" s="1" t="s">
-        <v>1087</v>
-      </c>
-      <c r="D706" s="13">
-        <v>640</v>
-      </c>
-      <c r="E706" s="13">
-        <v>635</v>
-      </c>
+        <v>1245</v>
+      </c>
+      <c r="D706" s="13"/>
+      <c r="E706" s="13"/>
       <c r="F706" s="17"/>
       <c r="G706" s="1"/>
       <c r="H706" s="1"/>
       <c r="I706" s="1"/>
-      <c r="J706" s="1">
-        <v>640</v>
-      </c>
-      <c r="K706" s="1">
-        <v>635</v>
-      </c>
-      <c r="L706" s="14">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="M706" s="14">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
+      <c r="J706" s="1"/>
+      <c r="K706" s="1"/>
+      <c r="L706" s="14"/>
+      <c r="M706" s="14"/>
       <c r="N706" s="1"/>
       <c r="O706" s="1"/>
       <c r="P706" s="1"/>
@@ -40847,7 +40833,7 @@
         <v>660</v>
       </c>
       <c r="E755" s="105">
-        <v>660</v>
+        <v>645</v>
       </c>
       <c r="F755" s="17"/>
       <c r="G755" s="1"/>
@@ -40865,7 +40851,7 @@
       </c>
       <c r="M755" s="116">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="N755" s="1"/>
       <c r="O755" s="1"/>

</xml_diff>

<commit_message>
chore: update Tinh BDS
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060B407A-5066-1C42-9DE5-C773C96DAA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3B46DD-3EA8-604E-8B63-C112571363F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3300" yWindow="760" windowWidth="27860" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5924,8 +5924,8 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A732" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E756" sqref="E756"/>
+      <pane ySplit="4" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D314" sqref="D314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -20554,7 +20554,7 @@
         <v>437</v>
       </c>
       <c r="D313" s="13">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="E313" s="13">
         <v>600</v>
@@ -20571,7 +20571,7 @@
       </c>
       <c r="L313" s="14">
         <f t="shared" si="8"/>
-        <v>-10</v>
+        <v>-15</v>
       </c>
       <c r="M313" s="14">
         <f t="shared" si="9"/>

</xml_diff>

<commit_message>
chore: update sponsor phone numbers
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3B46DD-3EA8-604E-8B63-C112571363F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D9FDAF-243A-0B46-BB14-337F72683590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3300" yWindow="760" windowWidth="27860" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="1321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="1321">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -5924,8 +5924,8 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D314" sqref="D314"/>
+      <pane ySplit="4" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E227" sqref="E227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16464,7 +16464,7 @@
         <v>650</v>
       </c>
       <c r="E226" s="13">
-        <v>620</v>
+        <v>640</v>
       </c>
       <c r="F226" s="21" t="s">
         <v>287</v>
@@ -16486,7 +16486,7 @@
       </c>
       <c r="M226" s="14">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N226" s="1"/>
       <c r="O226" s="1"/>
@@ -19061,34 +19061,18 @@
       </c>
       <c r="B281" s="14"/>
       <c r="C281" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="D281" s="13">
-        <v>650</v>
-      </c>
-      <c r="E281" s="13">
-        <v>645</v>
-      </c>
+        <v>1245</v>
+      </c>
+      <c r="D281" s="13"/>
+      <c r="E281" s="13"/>
       <c r="F281" s="15"/>
-      <c r="G281" s="12" t="s">
-        <v>152</v>
-      </c>
+      <c r="G281" s="12"/>
       <c r="H281" s="14"/>
       <c r="I281" s="14"/>
-      <c r="J281" s="16">
-        <v>650</v>
-      </c>
-      <c r="K281" s="16">
-        <v>645</v>
-      </c>
-      <c r="L281" s="14">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="M281" s="14">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
+      <c r="J281" s="16"/>
+      <c r="K281" s="16"/>
+      <c r="L281" s="14"/>
+      <c r="M281" s="14"/>
       <c r="N281" s="1"/>
       <c r="O281" s="1"/>
       <c r="P281" s="1"/>

</xml_diff>

<commit_message>
chore: update vu trong hieu 615
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163CB9B6-902D-1E4C-AC81-8F38AFED2F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8447C1D1-6A84-4E43-B389-CC66EF59D384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13960" yWindow="760" windowWidth="16480" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10520" yWindow="780" windowWidth="16480" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -5402,6 +5402,13 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5421,13 +5428,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6645,9 +6645,9 @@
   <dimension ref="A1:N998"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A409" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G36" sqref="G36"/>
-      <selection pane="bottomLeft" activeCell="C222" sqref="C222"/>
+      <selection pane="bottomLeft" activeCell="E435" sqref="E435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6664,15 +6664,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -6682,15 +6682,15 @@
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="134"/>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
+      <c r="B2" s="136"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -6725,10 +6725,10 @@
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="135" t="s">
+      <c r="D4" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="136"/>
+      <c r="E4" s="138"/>
       <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
@@ -12231,7 +12231,7 @@
       <c r="E222" s="96">
         <v>610</v>
       </c>
-      <c r="F222" s="142" t="s">
+      <c r="F222" s="134" t="s">
         <v>1572</v>
       </c>
       <c r="G222" s="67"/>
@@ -12331,7 +12331,7 @@
       <c r="E226" s="95">
         <v>640</v>
       </c>
-      <c r="F226" s="141" t="s">
+      <c r="F226" s="133" t="s">
         <v>1571</v>
       </c>
       <c r="G226" s="67"/>
@@ -17598,7 +17598,7 @@
         <v>560</v>
       </c>
       <c r="D435" s="97">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="E435" s="97">
         <v>610</v>
@@ -31363,14 +31363,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
@@ -31383,14 +31383,14 @@
       <c r="P1" s="10"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="137" t="s">
+      <c r="A2" s="139" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="138"/>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -31430,10 +31430,10 @@
       <c r="C4" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="139" t="s">
+      <c r="D4" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="140"/>
+      <c r="E4" s="142"/>
       <c r="F4" s="45" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
chore: update 3 members as ba suggests
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB19540-3B78-034C-8116-B6F285E178AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F143131-4FDB-404B-ADBD-D02926C6A5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21840" yWindow="29560" windowWidth="30440" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19560" yWindow="29560" windowWidth="30440" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -4911,13 +4911,13 @@
     <t xml:space="preserve">Kha Kỳ Hòa </t>
   </si>
   <si>
-    <t>Tạ Vạn Kim</t>
-  </si>
-  <si>
     <t>Quân PTSC</t>
   </si>
   <si>
     <t>Vị Titaha</t>
+  </si>
+  <si>
+    <t>Ta Vạn Kim</t>
   </si>
 </sst>
 </file>
@@ -6808,9 +6808,9 @@
   <dimension ref="A1:G1021"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A700" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A827" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G36" sqref="G36"/>
-      <selection pane="bottomLeft" activeCell="G717" sqref="G717"/>
+      <selection pane="bottomLeft" activeCell="G841" sqref="G841"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -19922,7 +19922,7 @@
       </c>
       <c r="B726" s="110"/>
       <c r="C726" s="112" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="D726" s="79">
         <v>590</v>
@@ -22193,7 +22193,7 @@
       </c>
       <c r="B853" s="119"/>
       <c r="C853" s="120" t="s">
-        <v>1625</v>
+        <v>1627</v>
       </c>
       <c r="D853" s="81">
         <v>605</v>
@@ -23893,7 +23893,7 @@
       </c>
       <c r="B949" s="123"/>
       <c r="C949" s="123" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="D949" s="78">
         <v>720</v>
@@ -25155,8 +25155,8 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6:F119"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26125,7 +26125,7 @@
         <v>600</v>
       </c>
       <c r="E37" s="43">
-        <v>730</v>
+        <v>590</v>
       </c>
       <c r="F37" s="44" t="s">
         <v>246</v>

</xml_diff>

<commit_message>
chore: update vu dam 745
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A8BC7B-5087-C446-A7FD-3AA1CF44B4B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1439433-01E5-314D-AA43-B8B52C466DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="760" windowWidth="24800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18360" yWindow="5840" windowWidth="24800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -6811,9 +6811,9 @@
   <dimension ref="A1:H1021"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A995" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G36" sqref="G36"/>
-      <selection pane="bottomLeft" activeCell="G1021" sqref="G1021"/>
+      <selection pane="bottomLeft" activeCell="E232" sqref="E232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11715,7 +11715,7 @@
         <v>257</v>
       </c>
       <c r="D232" s="81">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="E232" s="81">
         <v>740</v>

</xml_diff>

<commit_message>
chore: update dung dong duong
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA0A16A-9C01-8B40-93B1-FF4DF95EA0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA9486D-9998-714C-9C0B-23B67C6551BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="760" windowWidth="24800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5574,6 +5574,9 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5593,9 +5596,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6832,10 +6832,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1025"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A549" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G36" sqref="G36"/>
-      <selection pane="bottomLeft" activeCell="D274" sqref="D274"/>
+      <selection pane="bottomLeft" activeCell="F566" sqref="F566"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6851,28 +6851,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="127" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
+      <c r="A2" s="128" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="129"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -6894,10 +6894,10 @@
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="129" t="s">
+      <c r="D4" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="130"/>
+      <c r="E4" s="131"/>
       <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
@@ -18763,10 +18763,10 @@
         <v>739</v>
       </c>
       <c r="D566" s="79">
-        <v>580</v>
+        <v>600</v>
       </c>
       <c r="E566" s="79">
-        <v>580</v>
+        <v>600</v>
       </c>
       <c r="F566" s="57"/>
       <c r="G566" s="15">
@@ -20650,7 +20650,7 @@
       <c r="E655" s="77">
         <v>610</v>
       </c>
-      <c r="F655" s="135" t="s">
+      <c r="F655" s="127" t="s">
         <v>1631</v>
       </c>
       <c r="G655" s="15">
@@ -28325,14 +28325,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="132" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
@@ -28346,14 +28346,14 @@
       <c r="Q1" s="9"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="131" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="132"/>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="132"/>
+      <c r="A2" s="132" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="133"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="133"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
@@ -28395,10 +28395,10 @@
       <c r="C4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="133" t="s">
+      <c r="D4" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="134"/>
+      <c r="E4" s="135"/>
       <c r="F4" s="35" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
chore: update duong thinh phat
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA9486D-9998-714C-9C0B-23B67C6551BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D54E9D-6715-4E46-B841-4DC2AA60B454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="760" windowWidth="24800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6832,16 +6832,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1025"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A549" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A928" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G36" sqref="G36"/>
-      <selection pane="bottomLeft" activeCell="F566" sqref="F566"/>
+      <selection pane="bottomLeft" activeCell="D945" sqref="D945"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="2" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="26.33203125" style="2" customWidth="1"/>
     <col min="4" max="5" width="16.5" style="32" customWidth="1"/>
     <col min="6" max="7" width="16.33203125" style="2" customWidth="1"/>
@@ -8361,10 +8361,10 @@
         <v>84</v>
       </c>
       <c r="D73" s="79">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="E73" s="79">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="F73" s="56" t="s">
         <v>85</v>
@@ -23547,10 +23547,10 @@
         <v>1291</v>
       </c>
       <c r="D795" s="79">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="E795" s="79">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="F795" s="4"/>
       <c r="G795" s="15">
@@ -25456,13 +25456,13 @@
       </c>
       <c r="B887" s="111"/>
       <c r="C887" s="101" t="s">
-        <v>1443</v>
+        <v>1171</v>
       </c>
       <c r="D887" s="78">
-        <v>645</v>
+        <v>0</v>
       </c>
       <c r="E887" s="78">
-        <v>635</v>
+        <v>0</v>
       </c>
       <c r="F887" s="17"/>
       <c r="G887" s="15">
@@ -25871,7 +25871,7 @@
         <v>1467</v>
       </c>
       <c r="D907" s="85">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="E907" s="85">
         <v>620</v>
@@ -26653,7 +26653,7 @@
         <v>1522</v>
       </c>
       <c r="D944" s="85">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="E944" s="85">
         <v>615</v>

</xml_diff>

<commit_message>
chore: show all member with 1
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02463BC-CFC6-DA4E-A210-204C29F5CDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E1D0F6-4BB6-944B-96E8-447C33BA0980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="500" windowWidth="30940" windowHeight="26720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="30940" windowHeight="26720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -5657,6 +5657,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5676,10 +5680,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6916,10 +6916,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1083"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A1030" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A1026" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G36" sqref="G36"/>
-      <selection pane="bottomLeft" activeCell="F1053" sqref="F1053"/>
+      <selection pane="bottomLeft" activeCell="G1025" sqref="G1025:G1050"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6935,28 +6935,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="H1" s="143"/>
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="144"/>
+      <c r="H1" s="144"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="142" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="143"/>
+      <c r="A2" s="143" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -6978,10 +6978,10 @@
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="144" t="s">
+      <c r="D4" s="145" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="145"/>
+      <c r="E4" s="146"/>
       <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
@@ -28355,7 +28355,7 @@
         <v>1021</v>
       </c>
       <c r="B1026" s="102"/>
-      <c r="C1026" s="150" t="s">
+      <c r="C1026" s="142" t="s">
         <v>1631</v>
       </c>
       <c r="D1026" s="78">
@@ -28365,7 +28365,9 @@
         <v>600</v>
       </c>
       <c r="F1026" s="78"/>
-      <c r="G1026" s="14"/>
+      <c r="G1026" s="14">
+        <v>1</v>
+      </c>
       <c r="H1026" s="102"/>
     </row>
     <row r="1027" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28373,7 +28375,7 @@
         <v>1022</v>
       </c>
       <c r="B1027" s="102"/>
-      <c r="C1027" s="150" t="s">
+      <c r="C1027" s="142" t="s">
         <v>1632</v>
       </c>
       <c r="D1027" s="78">
@@ -28385,7 +28387,9 @@
       <c r="F1027" s="78" t="s">
         <v>1659</v>
       </c>
-      <c r="G1027" s="14"/>
+      <c r="G1027" s="14">
+        <v>1</v>
+      </c>
       <c r="H1027" s="102"/>
     </row>
     <row r="1028" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28393,7 +28397,7 @@
         <v>1023</v>
       </c>
       <c r="B1028" s="102"/>
-      <c r="C1028" s="150" t="s">
+      <c r="C1028" s="142" t="s">
         <v>1633</v>
       </c>
       <c r="D1028" s="78">
@@ -28403,7 +28407,9 @@
         <v>610</v>
       </c>
       <c r="F1028" s="78"/>
-      <c r="G1028" s="14"/>
+      <c r="G1028" s="14">
+        <v>1</v>
+      </c>
       <c r="H1028" s="102"/>
     </row>
     <row r="1029" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28411,7 +28417,7 @@
         <v>1024</v>
       </c>
       <c r="B1029" s="102"/>
-      <c r="C1029" s="150" t="s">
+      <c r="C1029" s="142" t="s">
         <v>1634</v>
       </c>
       <c r="D1029" s="78">
@@ -28421,7 +28427,9 @@
         <v>620</v>
       </c>
       <c r="F1029" s="78"/>
-      <c r="G1029" s="14"/>
+      <c r="G1029" s="14">
+        <v>1</v>
+      </c>
       <c r="H1029" s="102"/>
     </row>
     <row r="1030" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28429,7 +28437,7 @@
         <v>1025</v>
       </c>
       <c r="B1030" s="102"/>
-      <c r="C1030" s="150" t="s">
+      <c r="C1030" s="142" t="s">
         <v>1635</v>
       </c>
       <c r="D1030" s="78">
@@ -28439,7 +28447,9 @@
         <v>625</v>
       </c>
       <c r="F1030" s="78"/>
-      <c r="G1030" s="14"/>
+      <c r="G1030" s="14">
+        <v>1</v>
+      </c>
       <c r="H1030" s="102"/>
     </row>
     <row r="1031" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28447,7 +28457,7 @@
         <v>1026</v>
       </c>
       <c r="B1031" s="102"/>
-      <c r="C1031" s="150" t="s">
+      <c r="C1031" s="142" t="s">
         <v>1636</v>
       </c>
       <c r="D1031" s="78">
@@ -28457,7 +28467,9 @@
         <v>595</v>
       </c>
       <c r="F1031" s="78"/>
-      <c r="G1031" s="14"/>
+      <c r="G1031" s="14">
+        <v>1</v>
+      </c>
       <c r="H1031" s="102"/>
     </row>
     <row r="1032" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28465,7 +28477,7 @@
         <v>1027</v>
       </c>
       <c r="B1032" s="102"/>
-      <c r="C1032" s="150" t="s">
+      <c r="C1032" s="142" t="s">
         <v>1637</v>
       </c>
       <c r="D1032" s="78">
@@ -28477,7 +28489,9 @@
       <c r="F1032" s="78" t="s">
         <v>1660</v>
       </c>
-      <c r="G1032" s="14"/>
+      <c r="G1032" s="14">
+        <v>1</v>
+      </c>
       <c r="H1032" s="102"/>
     </row>
     <row r="1033" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28485,7 +28499,7 @@
         <v>1028</v>
       </c>
       <c r="B1033" s="102"/>
-      <c r="C1033" s="150" t="s">
+      <c r="C1033" s="142" t="s">
         <v>1638</v>
       </c>
       <c r="D1033" s="78">
@@ -28495,7 +28509,9 @@
         <v>590</v>
       </c>
       <c r="F1033" s="78"/>
-      <c r="G1033" s="14"/>
+      <c r="G1033" s="14">
+        <v>1</v>
+      </c>
       <c r="H1033" s="102"/>
     </row>
     <row r="1034" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28503,7 +28519,7 @@
         <v>1029</v>
       </c>
       <c r="B1034" s="102"/>
-      <c r="C1034" s="150" t="s">
+      <c r="C1034" s="142" t="s">
         <v>1639</v>
       </c>
       <c r="D1034" s="78">
@@ -28513,7 +28529,9 @@
         <v>600</v>
       </c>
       <c r="F1034" s="78"/>
-      <c r="G1034" s="14"/>
+      <c r="G1034" s="14">
+        <v>1</v>
+      </c>
       <c r="H1034" s="102"/>
     </row>
     <row r="1035" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28521,7 +28539,7 @@
         <v>1030</v>
       </c>
       <c r="B1035" s="102"/>
-      <c r="C1035" s="150" t="s">
+      <c r="C1035" s="142" t="s">
         <v>1640</v>
       </c>
       <c r="D1035" s="78">
@@ -28531,7 +28549,9 @@
         <v>600</v>
       </c>
       <c r="F1035" s="78"/>
-      <c r="G1035" s="14"/>
+      <c r="G1035" s="14">
+        <v>1</v>
+      </c>
       <c r="H1035" s="102"/>
     </row>
     <row r="1036" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28539,7 +28559,7 @@
         <v>1031</v>
       </c>
       <c r="B1036" s="102"/>
-      <c r="C1036" s="150" t="s">
+      <c r="C1036" s="142" t="s">
         <v>1641</v>
       </c>
       <c r="D1036" s="78">
@@ -28549,7 +28569,9 @@
         <v>600</v>
       </c>
       <c r="F1036" s="78"/>
-      <c r="G1036" s="14"/>
+      <c r="G1036" s="14">
+        <v>1</v>
+      </c>
       <c r="H1036" s="102"/>
     </row>
     <row r="1037" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28557,7 +28579,7 @@
         <v>1032</v>
       </c>
       <c r="B1037" s="102"/>
-      <c r="C1037" s="150" t="s">
+      <c r="C1037" s="142" t="s">
         <v>1642</v>
       </c>
       <c r="D1037" s="78">
@@ -28567,7 +28589,9 @@
         <v>610</v>
       </c>
       <c r="F1037" s="78"/>
-      <c r="G1037" s="14"/>
+      <c r="G1037" s="14">
+        <v>1</v>
+      </c>
       <c r="H1037" s="102"/>
     </row>
     <row r="1038" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28575,7 +28599,7 @@
         <v>1033</v>
       </c>
       <c r="B1038" s="102"/>
-      <c r="C1038" s="150" t="s">
+      <c r="C1038" s="142" t="s">
         <v>1643</v>
       </c>
       <c r="D1038" s="78">
@@ -28585,7 +28609,9 @@
         <v>610</v>
       </c>
       <c r="F1038" s="78"/>
-      <c r="G1038" s="14"/>
+      <c r="G1038" s="14">
+        <v>1</v>
+      </c>
       <c r="H1038" s="102"/>
     </row>
     <row r="1039" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28593,7 +28619,7 @@
         <v>1034</v>
       </c>
       <c r="B1039" s="102"/>
-      <c r="C1039" s="150" t="s">
+      <c r="C1039" s="142" t="s">
         <v>1644</v>
       </c>
       <c r="D1039" s="78">
@@ -28605,7 +28631,9 @@
       <c r="F1039" s="78" t="s">
         <v>1661</v>
       </c>
-      <c r="G1039" s="14"/>
+      <c r="G1039" s="14">
+        <v>1</v>
+      </c>
       <c r="H1039" s="102"/>
     </row>
     <row r="1040" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28613,7 +28641,7 @@
         <v>1035</v>
       </c>
       <c r="B1040" s="102"/>
-      <c r="C1040" s="150" t="s">
+      <c r="C1040" s="142" t="s">
         <v>1645</v>
       </c>
       <c r="D1040" s="78">
@@ -28625,7 +28653,9 @@
       <c r="F1040" s="78" t="s">
         <v>1662</v>
       </c>
-      <c r="G1040" s="14"/>
+      <c r="G1040" s="14">
+        <v>1</v>
+      </c>
       <c r="H1040" s="102"/>
     </row>
     <row r="1041" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28633,7 +28663,7 @@
         <v>1036</v>
       </c>
       <c r="B1041" s="102"/>
-      <c r="C1041" s="150" t="s">
+      <c r="C1041" s="142" t="s">
         <v>1646</v>
       </c>
       <c r="D1041" s="78">
@@ -28645,7 +28675,9 @@
       <c r="F1041" s="78" t="s">
         <v>1663</v>
       </c>
-      <c r="G1041" s="14"/>
+      <c r="G1041" s="14">
+        <v>1</v>
+      </c>
       <c r="H1041" s="102"/>
     </row>
     <row r="1042" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28653,7 +28685,7 @@
         <v>1037</v>
       </c>
       <c r="B1042" s="102"/>
-      <c r="C1042" s="150" t="s">
+      <c r="C1042" s="142" t="s">
         <v>1647</v>
       </c>
       <c r="D1042" s="78">
@@ -28663,7 +28695,9 @@
         <v>615</v>
       </c>
       <c r="F1042" s="78"/>
-      <c r="G1042" s="14"/>
+      <c r="G1042" s="14">
+        <v>1</v>
+      </c>
       <c r="H1042" s="102"/>
     </row>
     <row r="1043" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28671,7 +28705,7 @@
         <v>1038</v>
       </c>
       <c r="B1043" s="102"/>
-      <c r="C1043" s="150" t="s">
+      <c r="C1043" s="142" t="s">
         <v>1648</v>
       </c>
       <c r="D1043" s="78">
@@ -28681,7 +28715,9 @@
         <v>670</v>
       </c>
       <c r="F1043" s="78"/>
-      <c r="G1043" s="14"/>
+      <c r="G1043" s="14">
+        <v>1</v>
+      </c>
       <c r="H1043" s="102"/>
     </row>
     <row r="1044" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28689,7 +28725,7 @@
         <v>1039</v>
       </c>
       <c r="B1044" s="102"/>
-      <c r="C1044" s="150" t="s">
+      <c r="C1044" s="142" t="s">
         <v>1649</v>
       </c>
       <c r="D1044" s="78">
@@ -28699,7 +28735,9 @@
         <v>640</v>
       </c>
       <c r="F1044" s="78"/>
-      <c r="G1044" s="14"/>
+      <c r="G1044" s="14">
+        <v>1</v>
+      </c>
       <c r="H1044" s="102"/>
     </row>
     <row r="1045" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28707,7 +28745,7 @@
         <v>1040</v>
       </c>
       <c r="B1045" s="102"/>
-      <c r="C1045" s="150" t="s">
+      <c r="C1045" s="142" t="s">
         <v>1650</v>
       </c>
       <c r="D1045" s="78">
@@ -28717,7 +28755,9 @@
         <v>605</v>
       </c>
       <c r="F1045" s="78"/>
-      <c r="G1045" s="14"/>
+      <c r="G1045" s="14">
+        <v>1</v>
+      </c>
       <c r="H1045" s="102"/>
     </row>
     <row r="1046" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28725,7 +28765,7 @@
         <v>1041</v>
       </c>
       <c r="B1046" s="102"/>
-      <c r="C1046" s="150" t="s">
+      <c r="C1046" s="142" t="s">
         <v>1651</v>
       </c>
       <c r="D1046" s="78">
@@ -28735,7 +28775,9 @@
         <v>605</v>
       </c>
       <c r="F1046" s="78"/>
-      <c r="G1046" s="14"/>
+      <c r="G1046" s="14">
+        <v>1</v>
+      </c>
       <c r="H1046" s="102"/>
     </row>
     <row r="1047" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28743,7 +28785,7 @@
         <v>1042</v>
       </c>
       <c r="B1047" s="102"/>
-      <c r="C1047" s="150" t="s">
+      <c r="C1047" s="142" t="s">
         <v>1652</v>
       </c>
       <c r="D1047" s="78">
@@ -28755,7 +28797,9 @@
       <c r="F1047" s="78" t="s">
         <v>1664</v>
       </c>
-      <c r="G1047" s="14"/>
+      <c r="G1047" s="14">
+        <v>1</v>
+      </c>
       <c r="H1047" s="102"/>
     </row>
     <row r="1048" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28763,7 +28807,7 @@
         <v>1043</v>
       </c>
       <c r="B1048" s="102"/>
-      <c r="C1048" s="150" t="s">
+      <c r="C1048" s="142" t="s">
         <v>1653</v>
       </c>
       <c r="D1048" s="78">
@@ -28773,7 +28817,9 @@
         <v>600</v>
       </c>
       <c r="F1048" s="78"/>
-      <c r="G1048" s="14"/>
+      <c r="G1048" s="14">
+        <v>1</v>
+      </c>
       <c r="H1048" s="102"/>
     </row>
     <row r="1049" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28781,7 +28827,7 @@
         <v>1044</v>
       </c>
       <c r="B1049" s="102"/>
-      <c r="C1049" s="150" t="s">
+      <c r="C1049" s="142" t="s">
         <v>1654</v>
       </c>
       <c r="D1049" s="78">
@@ -28793,7 +28839,9 @@
       <c r="F1049" s="78" t="s">
         <v>1665</v>
       </c>
-      <c r="G1049" s="14"/>
+      <c r="G1049" s="14">
+        <v>1</v>
+      </c>
       <c r="H1049" s="102"/>
     </row>
     <row r="1050" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -28801,7 +28849,7 @@
         <v>1045</v>
       </c>
       <c r="B1050" s="102"/>
-      <c r="C1050" s="150" t="s">
+      <c r="C1050" s="142" t="s">
         <v>1655</v>
       </c>
       <c r="D1050" s="78">
@@ -28811,13 +28859,15 @@
         <v>735</v>
       </c>
       <c r="F1050" s="78"/>
-      <c r="G1050" s="14"/>
+      <c r="G1050" s="14">
+        <v>1</v>
+      </c>
       <c r="H1050" s="102"/>
     </row>
     <row r="1051" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1051" s="4"/>
       <c r="B1051" s="102"/>
-      <c r="C1051" s="150"/>
+      <c r="C1051" s="142"/>
       <c r="D1051" s="78"/>
       <c r="E1051" s="78"/>
       <c r="F1051" s="78"/>
@@ -29145,7 +29195,7 @@
       <c r="H1083" s="102"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Z+3Pe/WHvv9Eziq5osNQbLbawSpUidG7OXMDhtYjjffRL7d0Ic0M7of3ioPzQ8OHd4Hcu/XYoka91uMjGXxGoA==" saltValue="3Aji+WhIqeRMRJgwZMgJVw==" spinCount="100000" sheet="1" formatCells="0"/>
+  <sheetProtection formatCells="0"/>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
@@ -29184,7 +29234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A120" sqref="A120"/>
     </sheetView>
@@ -29202,14 +29252,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="147" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
+      <c r="B1" s="148"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
@@ -29223,14 +29273,14 @@
       <c r="Q1" s="8"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="146" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
+      <c r="A2" s="147" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -29272,10 +29322,10 @@
       <c r="C4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="148" t="s">
+      <c r="D4" s="149" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="149"/>
+      <c r="E4" s="150"/>
       <c r="F4" s="33" t="s">
         <v>6</v>
       </c>
@@ -49452,7 +49502,7 @@
       <c r="Q1000" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="eY6tBBLVZgp4UmPtbwFXqhlAMnWuNHn0STExwMRfDyEJAOhi3csCKczLwBb8Uj5HInMKYPd8OWnknwo+MBxICQ==" saltValue="yhrWgkGgsXueaqX1536IbQ==" spinCount="100000" sheet="1" formatCells="0"/>
+  <sheetProtection formatCells="0"/>
   <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>

</xml_diff>

<commit_message>
chore: update 3 members
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E1D0F6-4BB6-944B-96E8-447C33BA0980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8EFFC3-5C8B-604B-934C-FE6848D45FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="500" windowWidth="30940" windowHeight="26720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="1380" windowWidth="30940" windowHeight="26720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1720" uniqueCount="1666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="1668">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -5019,6 +5019,12 @@
   </si>
   <si>
     <t>0907569589</t>
+  </si>
+  <si>
+    <t>Luân Đồ Câu</t>
+  </si>
+  <si>
+    <t>0948985050</t>
   </si>
 </sst>
 </file>
@@ -5338,7 +5344,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
@@ -5680,6 +5686,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6916,10 +6926,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1083"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A1026" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A1009" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G36" sqref="G36"/>
-      <selection pane="bottomLeft" activeCell="G1025" sqref="G1025:G1050"/>
+      <selection pane="bottomLeft" activeCell="H1051" sqref="H1051"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -19800,7 +19810,7 @@
         <v>810</v>
       </c>
       <c r="D611" s="71">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="E611" s="71">
         <v>620</v>
@@ -24890,7 +24900,7 @@
         <v>1348</v>
       </c>
       <c r="D855" s="71">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="E855" s="71">
         <v>605</v>
@@ -27082,7 +27092,7 @@
         <v>1556</v>
       </c>
       <c r="D961" s="110">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="E961" s="110">
         <v>605</v>
@@ -28865,13 +28875,25 @@
       <c r="H1050" s="102"/>
     </row>
     <row r="1051" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1051" s="4"/>
+      <c r="A1051" s="4">
+        <v>1045</v>
+      </c>
       <c r="B1051" s="102"/>
-      <c r="C1051" s="142"/>
-      <c r="D1051" s="78"/>
-      <c r="E1051" s="78"/>
-      <c r="F1051" s="78"/>
-      <c r="G1051" s="14"/>
+      <c r="C1051" s="142" t="s">
+        <v>1666</v>
+      </c>
+      <c r="D1051" s="78">
+        <v>625</v>
+      </c>
+      <c r="E1051" s="78">
+        <v>615</v>
+      </c>
+      <c r="F1051" s="151" t="s">
+        <v>1667</v>
+      </c>
+      <c r="G1051" s="14">
+        <v>1</v>
+      </c>
       <c r="H1051" s="102"/>
     </row>
     <row r="1052" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -29234,7 +29256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A120" sqref="A120"/>
     </sheetView>

</xml_diff>

<commit_message>
chore: update score at home
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8EFFC3-5C8B-604B-934C-FE6848D45FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4005445-EA14-5D42-9B90-85BC6975ACAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="1380" windowWidth="30940" windowHeight="26720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="760" windowWidth="24800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="1668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1733" uniqueCount="1679">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -5025,6 +5025,39 @@
   </si>
   <si>
     <t>0948985050</t>
+  </si>
+  <si>
+    <t>Tân Menulife</t>
+  </si>
+  <si>
+    <t>Việt Tôn</t>
+  </si>
+  <si>
+    <t>Tiên Phạm VT</t>
+  </si>
+  <si>
+    <t>Phương Vy VT</t>
+  </si>
+  <si>
+    <t>Lê Na</t>
+  </si>
+  <si>
+    <t>BS Khánh</t>
+  </si>
+  <si>
+    <t>0903678216</t>
+  </si>
+  <si>
+    <t>BS Phong</t>
+  </si>
+  <si>
+    <t>Minh Lotus</t>
+  </si>
+  <si>
+    <t>Dũng Viettel</t>
+  </si>
+  <si>
+    <t>Can ĐL</t>
   </si>
 </sst>
 </file>
@@ -5667,6 +5700,10 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5686,10 +5723,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6927,9 +6960,9 @@
   <dimension ref="A1:H1083"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A1009" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A1032" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G36" sqref="G36"/>
-      <selection pane="bottomLeft" activeCell="H1051" sqref="H1051"/>
+      <selection pane="bottomLeft" activeCell="C1062" sqref="C1062"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6945,28 +6978,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
+      <c r="E1" s="145"/>
+      <c r="F1" s="145"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="143" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="144"/>
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="G2" s="144"/>
-      <c r="H2" s="144"/>
+      <c r="A2" s="144" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="145"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -6988,10 +7021,10 @@
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="145" t="s">
+      <c r="D4" s="146" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="146"/>
+      <c r="E4" s="147"/>
       <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
@@ -7441,7 +7474,7 @@
         <v>33</v>
       </c>
       <c r="D25" s="71">
-        <v>615</v>
+        <v>620</v>
       </c>
       <c r="E25" s="71">
         <v>615</v>
@@ -8819,7 +8852,7 @@
         <v>107</v>
       </c>
       <c r="D90" s="72">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="E90" s="72">
         <v>600</v>
@@ -23924,7 +23957,7 @@
         <v>1304</v>
       </c>
       <c r="D809" s="73">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="E809" s="73">
         <v>615</v>
@@ -24606,7 +24639,7 @@
         <v>1335</v>
       </c>
       <c r="D841" s="73">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="E841" s="73">
         <v>615</v>
@@ -25290,7 +25323,7 @@
         <v>1374</v>
       </c>
       <c r="D874" s="71">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="E874" s="71">
         <v>625</v>
@@ -25452,7 +25485,7 @@
         <v>1438</v>
       </c>
       <c r="D882" s="71">
-        <v>645</v>
+        <v>655</v>
       </c>
       <c r="E882" s="71">
         <v>645</v>
@@ -25924,7 +25957,7 @@
         <v>1465</v>
       </c>
       <c r="D905" s="107">
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="E905" s="107">
         <v>600</v>
@@ -26552,7 +26585,7 @@
         <v>1506</v>
       </c>
       <c r="D935" s="107">
-        <v>585</v>
+        <v>595</v>
       </c>
       <c r="E935" s="107">
         <v>585</v>
@@ -27760,10 +27793,10 @@
         <v>1593</v>
       </c>
       <c r="D994" s="78">
+        <v>635</v>
+      </c>
+      <c r="E994" s="78">
         <v>620</v>
-      </c>
-      <c r="E994" s="78">
-        <v>610</v>
       </c>
       <c r="F994" s="4"/>
       <c r="G994" s="14">
@@ -27974,10 +28007,10 @@
         <v>1604</v>
       </c>
       <c r="D1005" s="78">
-        <v>600</v>
+        <v>615</v>
       </c>
       <c r="E1005" s="78">
-        <v>590</v>
+        <v>605</v>
       </c>
       <c r="F1005" s="4"/>
       <c r="G1005" s="14">
@@ -28888,7 +28921,7 @@
       <c r="E1051" s="78">
         <v>615</v>
       </c>
-      <c r="F1051" s="151" t="s">
+      <c r="F1051" s="143" t="s">
         <v>1667</v>
       </c>
       <c r="G1051" s="14">
@@ -28897,73 +28930,145 @@
       <c r="H1051" s="102"/>
     </row>
     <row r="1052" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1052" s="102"/>
+      <c r="A1052" s="4">
+        <v>1046</v>
+      </c>
       <c r="B1052" s="102"/>
-      <c r="C1052" s="102"/>
-      <c r="D1052" s="117"/>
-      <c r="E1052" s="117"/>
-      <c r="F1052" s="102"/>
-      <c r="G1052" s="102"/>
+      <c r="C1052" s="142" t="s">
+        <v>1668</v>
+      </c>
+      <c r="D1052" s="78">
+        <v>625</v>
+      </c>
+      <c r="E1052" s="78">
+        <v>620</v>
+      </c>
+      <c r="F1052" s="143"/>
+      <c r="G1052" s="14">
+        <v>1</v>
+      </c>
       <c r="H1052" s="102"/>
     </row>
     <row r="1053" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1053" s="102"/>
+      <c r="A1053" s="4">
+        <v>1047</v>
+      </c>
       <c r="B1053" s="102"/>
-      <c r="C1053" s="102"/>
-      <c r="D1053" s="117"/>
-      <c r="E1053" s="117"/>
-      <c r="F1053" s="102"/>
-      <c r="G1053" s="102"/>
+      <c r="C1053" s="142" t="s">
+        <v>1669</v>
+      </c>
+      <c r="D1053" s="78">
+        <v>595</v>
+      </c>
+      <c r="E1053" s="78">
+        <v>595</v>
+      </c>
+      <c r="F1053" s="143"/>
+      <c r="G1053" s="14">
+        <v>1</v>
+      </c>
       <c r="H1053" s="102"/>
     </row>
     <row r="1054" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1054" s="102"/>
+      <c r="A1054" s="4">
+        <v>1048</v>
+      </c>
       <c r="B1054" s="102"/>
-      <c r="C1054" s="102"/>
-      <c r="D1054" s="117"/>
-      <c r="E1054" s="117"/>
-      <c r="F1054" s="102"/>
-      <c r="G1054" s="102"/>
+      <c r="C1054" s="142" t="s">
+        <v>1673</v>
+      </c>
+      <c r="D1054" s="78">
+        <v>635</v>
+      </c>
+      <c r="E1054" s="78">
+        <v>635</v>
+      </c>
+      <c r="F1054" s="143" t="s">
+        <v>1674</v>
+      </c>
+      <c r="G1054" s="14">
+        <v>1</v>
+      </c>
       <c r="H1054" s="102"/>
     </row>
     <row r="1055" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1055" s="102"/>
+      <c r="A1055" s="4">
+        <v>1049</v>
+      </c>
       <c r="B1055" s="102"/>
-      <c r="C1055" s="102"/>
-      <c r="D1055" s="117"/>
-      <c r="E1055" s="117"/>
-      <c r="F1055" s="102"/>
-      <c r="G1055" s="102"/>
+      <c r="C1055" s="142" t="s">
+        <v>1675</v>
+      </c>
+      <c r="D1055" s="78">
+        <v>645</v>
+      </c>
+      <c r="E1055" s="78">
+        <v>645</v>
+      </c>
+      <c r="F1055" s="143"/>
+      <c r="G1055" s="14">
+        <v>1</v>
+      </c>
       <c r="H1055" s="102"/>
     </row>
     <row r="1056" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1056" s="102"/>
+      <c r="A1056" s="4">
+        <v>1050</v>
+      </c>
       <c r="B1056" s="102"/>
-      <c r="C1056" s="102"/>
-      <c r="D1056" s="117"/>
-      <c r="E1056" s="117"/>
-      <c r="F1056" s="102"/>
-      <c r="G1056" s="102"/>
+      <c r="C1056" s="142" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D1056" s="78">
+        <v>635</v>
+      </c>
+      <c r="E1056" s="78">
+        <v>635</v>
+      </c>
+      <c r="F1056" s="143"/>
+      <c r="G1056" s="14">
+        <v>1</v>
+      </c>
       <c r="H1056" s="102"/>
     </row>
     <row r="1057" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1057" s="102"/>
+      <c r="A1057" s="4">
+        <v>1051</v>
+      </c>
       <c r="B1057" s="102"/>
-      <c r="C1057" s="102"/>
-      <c r="D1057" s="117"/>
-      <c r="E1057" s="117"/>
-      <c r="F1057" s="102"/>
-      <c r="G1057" s="102"/>
+      <c r="C1057" s="142" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D1057" s="78">
+        <v>625</v>
+      </c>
+      <c r="E1057" s="78">
+        <v>625</v>
+      </c>
+      <c r="F1057" s="143"/>
+      <c r="G1057" s="14">
+        <v>1</v>
+      </c>
       <c r="H1057" s="102"/>
     </row>
     <row r="1058" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1058" s="102"/>
+      <c r="A1058" s="4">
+        <v>1052</v>
+      </c>
       <c r="B1058" s="102"/>
-      <c r="C1058" s="102"/>
-      <c r="D1058" s="117"/>
-      <c r="E1058" s="117"/>
-      <c r="F1058" s="102"/>
-      <c r="G1058" s="102"/>
+      <c r="C1058" s="142" t="s">
+        <v>1678</v>
+      </c>
+      <c r="D1058" s="78">
+        <v>595</v>
+      </c>
+      <c r="E1058" s="78">
+        <v>595</v>
+      </c>
+      <c r="F1058" s="143"/>
+      <c r="G1058" s="14">
+        <v>1</v>
+      </c>
       <c r="H1058" s="102"/>
     </row>
     <row r="1059" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -29223,7 +29328,7 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="D4:E4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1:C3 C1052:C1048576">
+  <conditionalFormatting sqref="C1:C3 C1059:C1048576">
     <cfRule type="duplicateValues" dxfId="6" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C5">
@@ -29241,7 +29346,7 @@
   <conditionalFormatting sqref="C967:C1021">
     <cfRule type="duplicateValues" dxfId="1" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1022:C1051">
+  <conditionalFormatting sqref="C1022:C1058">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -29256,15 +29361,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A120" sqref="A120"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="9" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="26.33203125" style="9" customWidth="1"/>
     <col min="4" max="5" width="16.5" style="9" customWidth="1"/>
     <col min="6" max="7" width="16.33203125" style="9" customWidth="1"/>
@@ -29274,14 +29379,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="148" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="148"/>
-      <c r="C1" s="148"/>
-      <c r="D1" s="148"/>
-      <c r="E1" s="148"/>
-      <c r="F1" s="148"/>
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
@@ -29295,14 +29400,14 @@
       <c r="Q1" s="8"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="147" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
-      <c r="F2" s="148"/>
+      <c r="A2" s="148" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -29344,10 +29449,10 @@
       <c r="C4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="149" t="s">
+      <c r="D4" s="150" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="150"/>
+      <c r="E4" s="151"/>
       <c r="F4" s="33" t="s">
         <v>6</v>
       </c>
@@ -32785,13 +32890,23 @@
       <c r="Q119" s="8"/>
     </row>
     <row r="120" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="4"/>
+      <c r="A120" s="37">
+        <v>115</v>
+      </c>
       <c r="B120" s="4"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="7"/>
-      <c r="E120" s="7"/>
-      <c r="F120" s="4"/>
-      <c r="G120" s="4"/>
+      <c r="C120" s="1" t="s">
+        <v>1670</v>
+      </c>
+      <c r="D120" s="7">
+        <v>580</v>
+      </c>
+      <c r="E120" s="7">
+        <v>580</v>
+      </c>
+      <c r="F120" s="14"/>
+      <c r="G120" s="34">
+        <v>1</v>
+      </c>
       <c r="H120" s="8"/>
       <c r="I120" s="8"/>
       <c r="J120" s="8"/>
@@ -32804,13 +32919,23 @@
       <c r="Q120" s="8"/>
     </row>
     <row r="121" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="4"/>
+      <c r="A121" s="37">
+        <v>116</v>
+      </c>
       <c r="B121" s="4"/>
-      <c r="C121" s="4"/>
-      <c r="D121" s="7"/>
-      <c r="E121" s="7"/>
+      <c r="C121" s="1" t="s">
+        <v>1671</v>
+      </c>
+      <c r="D121" s="7">
+        <v>590</v>
+      </c>
+      <c r="E121" s="7">
+        <v>590</v>
+      </c>
       <c r="F121" s="14"/>
-      <c r="G121" s="14"/>
+      <c r="G121" s="34">
+        <v>1</v>
+      </c>
       <c r="H121" s="8"/>
       <c r="I121" s="8"/>
       <c r="J121" s="8"/>
@@ -32823,13 +32948,23 @@
       <c r="Q121" s="8"/>
     </row>
     <row r="122" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="4"/>
+      <c r="A122" s="37">
+        <v>117</v>
+      </c>
       <c r="B122" s="4"/>
-      <c r="C122" s="4"/>
-      <c r="D122" s="7"/>
-      <c r="E122" s="7"/>
+      <c r="C122" s="1" t="s">
+        <v>1672</v>
+      </c>
+      <c r="D122" s="7">
+        <v>575</v>
+      </c>
+      <c r="E122" s="7">
+        <v>575</v>
+      </c>
       <c r="F122" s="14"/>
-      <c r="G122" s="14"/>
+      <c r="G122" s="34">
+        <v>1</v>
+      </c>
       <c r="H122" s="8"/>
       <c r="I122" s="8"/>
       <c r="J122" s="8"/>
@@ -32842,13 +32977,13 @@
       <c r="Q122" s="8"/>
     </row>
     <row r="123" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="4"/>
+      <c r="A123" s="37"/>
       <c r="B123" s="4"/>
-      <c r="C123" s="4"/>
+      <c r="C123" s="1"/>
       <c r="D123" s="7"/>
       <c r="E123" s="7"/>
-      <c r="F123" s="4"/>
-      <c r="G123" s="4"/>
+      <c r="F123" s="14"/>
+      <c r="G123" s="34"/>
       <c r="H123" s="8"/>
       <c r="I123" s="8"/>
       <c r="J123" s="8"/>
@@ -32861,13 +32996,13 @@
       <c r="Q123" s="8"/>
     </row>
     <row r="124" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="4"/>
+      <c r="A124" s="37"/>
       <c r="B124" s="4"/>
-      <c r="C124" s="4"/>
+      <c r="C124" s="1"/>
       <c r="D124" s="7"/>
       <c r="E124" s="7"/>
-      <c r="F124" s="4"/>
-      <c r="G124" s="4"/>
+      <c r="F124" s="14"/>
+      <c r="G124" s="34"/>
       <c r="H124" s="8"/>
       <c r="I124" s="8"/>
       <c r="J124" s="8"/>
@@ -32880,13 +33015,13 @@
       <c r="Q124" s="8"/>
     </row>
     <row r="125" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="4"/>
+      <c r="A125" s="37"/>
       <c r="B125" s="4"/>
-      <c r="C125" s="4"/>
+      <c r="C125" s="1"/>
       <c r="D125" s="7"/>
       <c r="E125" s="7"/>
       <c r="F125" s="14"/>
-      <c r="G125" s="14"/>
+      <c r="G125" s="34"/>
       <c r="H125" s="8"/>
       <c r="I125" s="8"/>
       <c r="J125" s="8"/>
@@ -32899,13 +33034,13 @@
       <c r="Q125" s="8"/>
     </row>
     <row r="126" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="4"/>
+      <c r="A126" s="37"/>
       <c r="B126" s="4"/>
-      <c r="C126" s="4"/>
+      <c r="C126" s="1"/>
       <c r="D126" s="7"/>
       <c r="E126" s="7"/>
       <c r="F126" s="14"/>
-      <c r="G126" s="14"/>
+      <c r="G126" s="34"/>
       <c r="H126" s="8"/>
       <c r="I126" s="8"/>
       <c r="J126" s="8"/>

</xml_diff>

<commit_message>
chore: update stt 720
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF1F113-C512-A04D-B40B-98DBA3E0778F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0274213F-1D92-324A-839D-2C43BD6CCCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="760" windowWidth="24800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28620" yWindow="8480" windowWidth="24800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -6960,9 +6960,9 @@
   <dimension ref="A1:H1083"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A1032" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A711" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G36" sqref="G36"/>
-      <selection pane="bottomLeft" activeCell="E1054" sqref="E1054"/>
+      <selection pane="bottomLeft" activeCell="D726" sqref="D726"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -22223,7 +22223,7 @@
         <v>1199</v>
       </c>
       <c r="D725" s="73">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="E725" s="73">
         <v>600</v>

</xml_diff>

<commit_message>
chore: update Luyen female score
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1330D46B-6EC6-AA49-86D7-2B8CF4A88255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47B7049-CDBD-F348-898C-D0BECE353B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40940" yWindow="3840" windowWidth="19580" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -7011,7 +7011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K1105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1074" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A1074" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C1102" sqref="C1102"/>
     </sheetView>
   </sheetViews>
@@ -36687,9 +36687,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A65" sqref="A65"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -37743,10 +37743,10 @@
         <v>913</v>
       </c>
       <c r="D33" s="112">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="E33" s="112">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="F33" s="15"/>
       <c r="G33" s="113">

</xml_diff>

<commit_message>
chore: update tuan long xuyen
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E613174-A81E-A644-B738-86337FAC775D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60223602-2487-1146-80AB-F1C26CFD17B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7008,8 +7008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K1105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1080" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D1096" sqref="D1096"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -36548,7 +36548,7 @@
         <v>1713</v>
       </c>
       <c r="D1096" s="98">
-        <v>685</v>
+        <v>670</v>
       </c>
       <c r="E1096" s="98">
         <v>670</v>

</xml_diff>

<commit_message>
Revert "chore: update banners"
This reverts commit 5450b93e1bf6313af5fee66117209da1bd225ef2.
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10161A1-C3CC-FC41-8EDB-F42CBBB81D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F316768-91D4-2349-AAE4-265AAD283CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1834" uniqueCount="1773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="1772">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -5259,6 +5259,9 @@
     <t>Hoài Cảng LX</t>
   </si>
   <si>
+    <t>Vũ Jimmu</t>
+  </si>
+  <si>
     <t>Nguyễn Dũng</t>
   </si>
   <si>
@@ -5380,12 +5383,6 @@
   </si>
   <si>
     <t>0334113399</t>
-  </si>
-  <si>
-    <t>Nhàn Cấp Nước</t>
-  </si>
-  <si>
-    <t>Vũ Jimmy</t>
   </si>
 </sst>
 </file>
@@ -6001,6 +5998,32 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -6033,49 +6056,13 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bình thường 2" xfId="2" xr:uid="{2DBE829A-806A-A246-9A23-241A22DA22A4}"/>
     <cellStyle name="Bình thường 3" xfId="1" xr:uid="{ABA3F074-F600-1940-87D2-1B8571A799F2}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -7312,10 +7299,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L1134"/>
+  <dimension ref="A1:L1133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1107" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C1119" sqref="C1119"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1115" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="K1128" sqref="K1128:L1133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7335,30 +7322,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
       <c r="K1" s="25"/>
       <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="127" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
+      <c r="A2" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
       <c r="K2" s="25"/>
       <c r="L2" s="25"/>
     </row>
@@ -7384,10 +7371,10 @@
       <c r="C4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="129" t="s">
+      <c r="D4" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="130"/>
+      <c r="E4" s="118"/>
       <c r="F4" s="49" t="s">
         <v>6</v>
       </c>
@@ -7397,10 +7384,10 @@
       <c r="H4" s="31" t="s">
         <v>1415</v>
       </c>
-      <c r="K4" s="131" t="s">
+      <c r="K4" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="132"/>
+      <c r="L4" s="120"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="48"/>
@@ -10959,7 +10946,7 @@
         <v>585</v>
       </c>
       <c r="F117" s="81" t="s">
-        <v>1770</v>
+        <v>1771</v>
       </c>
       <c r="G117" s="15">
         <v>1</v>
@@ -16888,7 +16875,7 @@
       </c>
       <c r="B305" s="51"/>
       <c r="C305" s="52" t="s">
-        <v>1762</v>
+        <v>1763</v>
       </c>
       <c r="D305" s="75">
         <f t="shared" si="8"/>
@@ -17775,8 +17762,8 @@
         <v>329</v>
       </c>
       <c r="B334" s="51"/>
-      <c r="C334" s="118" t="s">
-        <v>1760</v>
+      <c r="C334" s="128" t="s">
+        <v>1761</v>
       </c>
       <c r="D334" s="75">
         <f t="shared" si="10"/>
@@ -34145,8 +34132,8 @@
         <v>856</v>
       </c>
       <c r="B861" s="53"/>
-      <c r="C861" s="125" t="s">
-        <v>1763</v>
+      <c r="C861" s="135" t="s">
+        <v>1764</v>
       </c>
       <c r="D861" s="75">
         <v>615</v>
@@ -37733,14 +37720,14 @@
         <v>972</v>
       </c>
       <c r="B977" s="1"/>
-      <c r="C977" s="116" t="s">
-        <v>1759</v>
-      </c>
-      <c r="D977" s="117">
+      <c r="C977" s="126" t="s">
+        <v>1760</v>
+      </c>
+      <c r="D977" s="127">
         <f t="shared" si="30"/>
         <v>610</v>
       </c>
-      <c r="E977" s="117">
+      <c r="E977" s="127">
         <f t="shared" si="31"/>
         <v>610</v>
       </c>
@@ -41861,7 +41848,7 @@
       </c>
       <c r="B1115" s="59"/>
       <c r="C1115" s="69" t="s">
-        <v>1772</v>
+        <v>1730</v>
       </c>
       <c r="D1115" s="75">
         <v>660</v>
@@ -41889,7 +41876,7 @@
       </c>
       <c r="B1116" s="59"/>
       <c r="C1116" s="69" t="s">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="D1116" s="75">
         <v>650</v>
@@ -41917,7 +41904,7 @@
       </c>
       <c r="B1117" s="59"/>
       <c r="C1117" s="69" t="s">
-        <v>1731</v>
+        <v>1732</v>
       </c>
       <c r="D1117" s="75">
         <v>605</v>
@@ -41945,7 +41932,7 @@
       </c>
       <c r="B1118" s="59"/>
       <c r="C1118" s="69" t="s">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="D1118" s="75">
         <v>625</v>
@@ -41973,7 +41960,7 @@
       </c>
       <c r="B1119" s="59"/>
       <c r="C1119" s="69" t="s">
-        <v>1748</v>
+        <v>1749</v>
       </c>
       <c r="D1119" s="75">
         <v>590</v>
@@ -42001,7 +41988,7 @@
       </c>
       <c r="B1120" s="59"/>
       <c r="C1120" s="69" t="s">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="D1120" s="75">
         <v>610</v>
@@ -42029,7 +42016,7 @@
       </c>
       <c r="B1121" s="59"/>
       <c r="C1121" s="69" t="s">
-        <v>1750</v>
+        <v>1751</v>
       </c>
       <c r="D1121" s="75">
         <v>610</v>
@@ -42057,7 +42044,7 @@
       </c>
       <c r="B1122" s="59"/>
       <c r="C1122" s="69" t="s">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="D1122" s="75">
         <v>605</v>
@@ -42085,7 +42072,7 @@
       </c>
       <c r="B1123" s="59"/>
       <c r="C1123" s="69" t="s">
-        <v>1752</v>
+        <v>1753</v>
       </c>
       <c r="D1123" s="75">
         <v>585</v>
@@ -42113,7 +42100,7 @@
       </c>
       <c r="B1124" s="59"/>
       <c r="C1124" s="69" t="s">
-        <v>1753</v>
+        <v>1754</v>
       </c>
       <c r="D1124" s="75">
         <v>600</v>
@@ -42141,7 +42128,7 @@
       </c>
       <c r="B1125" s="59"/>
       <c r="C1125" s="69" t="s">
-        <v>1754</v>
+        <v>1755</v>
       </c>
       <c r="D1125" s="75">
         <v>700</v>
@@ -42169,7 +42156,7 @@
       </c>
       <c r="B1126" s="59"/>
       <c r="C1126" s="69" t="s">
-        <v>1755</v>
+        <v>1756</v>
       </c>
       <c r="D1126" s="75">
         <v>660</v>
@@ -42197,7 +42184,7 @@
       </c>
       <c r="B1127" s="59"/>
       <c r="C1127" s="69" t="s">
-        <v>1756</v>
+        <v>1757</v>
       </c>
       <c r="D1127" s="75">
         <v>710</v>
@@ -42225,7 +42212,7 @@
       </c>
       <c r="B1128" s="59"/>
       <c r="C1128" s="69" t="s">
-        <v>1757</v>
+        <v>1758</v>
       </c>
       <c r="D1128" s="75">
         <v>690</v>
@@ -42251,27 +42238,27 @@
       <c r="A1129" s="2">
         <v>1123</v>
       </c>
-      <c r="B1129" s="119"/>
-      <c r="C1129" s="120" t="s">
-        <v>1761</v>
-      </c>
-      <c r="D1129" s="121">
+      <c r="B1129" s="129"/>
+      <c r="C1129" s="130" t="s">
+        <v>1762</v>
+      </c>
+      <c r="D1129" s="131">
         <v>595</v>
       </c>
-      <c r="E1129" s="121">
+      <c r="E1129" s="131">
         <v>590</v>
       </c>
-      <c r="F1129" s="119"/>
+      <c r="F1129" s="129"/>
       <c r="G1129" s="15">
         <v>1</v>
       </c>
-      <c r="H1129" s="122"/>
-      <c r="I1129" s="123"/>
-      <c r="J1129" s="123"/>
-      <c r="K1129" s="124">
+      <c r="H1129" s="132"/>
+      <c r="I1129" s="133"/>
+      <c r="J1129" s="133"/>
+      <c r="K1129" s="134">
         <v>595</v>
       </c>
-      <c r="L1129" s="124">
+      <c r="L1129" s="134">
         <v>590</v>
       </c>
     </row>
@@ -42279,27 +42266,27 @@
       <c r="A1130" s="2">
         <v>1124</v>
       </c>
-      <c r="B1130" s="119"/>
-      <c r="C1130" s="120" t="s">
-        <v>1765</v>
-      </c>
-      <c r="D1130" s="121">
+      <c r="B1130" s="129"/>
+      <c r="C1130" s="130" t="s">
+        <v>1766</v>
+      </c>
+      <c r="D1130" s="131">
         <v>645</v>
       </c>
-      <c r="E1130" s="121">
+      <c r="E1130" s="131">
         <v>640</v>
       </c>
-      <c r="F1130" s="119"/>
+      <c r="F1130" s="129"/>
       <c r="G1130" s="15">
         <v>1</v>
       </c>
-      <c r="H1130" s="122"/>
-      <c r="I1130" s="123"/>
-      <c r="J1130" s="123"/>
-      <c r="K1130" s="124">
+      <c r="H1130" s="132"/>
+      <c r="I1130" s="133"/>
+      <c r="J1130" s="133"/>
+      <c r="K1130" s="134">
         <v>645</v>
       </c>
-      <c r="L1130" s="124">
+      <c r="L1130" s="134">
         <v>640</v>
       </c>
     </row>
@@ -42307,27 +42294,27 @@
       <c r="A1131" s="2">
         <v>1125</v>
       </c>
-      <c r="B1131" s="119"/>
-      <c r="C1131" s="120" t="s">
-        <v>1764</v>
-      </c>
-      <c r="D1131" s="121">
+      <c r="B1131" s="129"/>
+      <c r="C1131" s="130" t="s">
+        <v>1765</v>
+      </c>
+      <c r="D1131" s="131">
         <v>620</v>
       </c>
-      <c r="E1131" s="121">
+      <c r="E1131" s="131">
         <v>610</v>
       </c>
-      <c r="F1131" s="119"/>
+      <c r="F1131" s="129"/>
       <c r="G1131" s="15">
         <v>1</v>
       </c>
-      <c r="H1131" s="122"/>
-      <c r="I1131" s="123"/>
-      <c r="J1131" s="123"/>
-      <c r="K1131" s="124">
+      <c r="H1131" s="132"/>
+      <c r="I1131" s="133"/>
+      <c r="J1131" s="133"/>
+      <c r="K1131" s="134">
         <v>620</v>
       </c>
-      <c r="L1131" s="124">
+      <c r="L1131" s="134">
         <v>610</v>
       </c>
     </row>
@@ -42335,81 +42322,55 @@
       <c r="A1132" s="2">
         <v>1126</v>
       </c>
-      <c r="B1132" s="119"/>
-      <c r="C1132" s="120" t="s">
-        <v>1766</v>
-      </c>
-      <c r="D1132" s="121">
+      <c r="B1132" s="129"/>
+      <c r="C1132" s="130" t="s">
+        <v>1767</v>
+      </c>
+      <c r="D1132" s="131">
         <v>600</v>
       </c>
-      <c r="E1132" s="121">
+      <c r="E1132" s="131">
         <v>595</v>
       </c>
-      <c r="F1132" s="119"/>
+      <c r="F1132" s="129"/>
       <c r="G1132" s="15">
         <v>1</v>
       </c>
-      <c r="H1132" s="122"/>
-      <c r="I1132" s="123"/>
-      <c r="J1132" s="123"/>
-      <c r="K1132" s="124">
+      <c r="H1132" s="132"/>
+      <c r="I1132" s="133"/>
+      <c r="J1132" s="133"/>
+      <c r="K1132" s="134">
         <v>600</v>
       </c>
-      <c r="L1132" s="124">
+      <c r="L1132" s="134">
         <v>595</v>
       </c>
     </row>
     <row r="1133" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1133" s="2">
-        <v>1267</v>
-      </c>
-      <c r="B1133" s="119"/>
-      <c r="C1133" s="120" t="s">
-        <v>1771</v>
-      </c>
-      <c r="D1133" s="121">
-        <v>645</v>
-      </c>
-      <c r="E1133" s="121"/>
-      <c r="F1133" s="119"/>
+      <c r="A1133" s="114">
+        <v>1136</v>
+      </c>
+      <c r="B1133" s="59"/>
+      <c r="C1133" s="125" t="s">
+        <v>1759</v>
+      </c>
+      <c r="D1133" s="104">
+        <v>605</v>
+      </c>
+      <c r="E1133" s="104">
+        <v>600</v>
+      </c>
+      <c r="F1133" s="59"/>
       <c r="G1133" s="15">
         <v>1</v>
       </c>
-      <c r="H1133" s="122"/>
-      <c r="I1133" s="123"/>
-      <c r="J1133" s="123"/>
-      <c r="K1133" s="124">
-        <v>600</v>
-      </c>
-      <c r="L1133" s="124">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="1134" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1134" s="114">
-        <v>1136</v>
-      </c>
-      <c r="B1134" s="59"/>
-      <c r="C1134" s="115" t="s">
-        <v>1758</v>
-      </c>
-      <c r="D1134" s="104">
+      <c r="H1133" s="26"/>
+      <c r="I1133" s="107"/>
+      <c r="J1133" s="107"/>
+      <c r="K1133" s="27">
         <v>605</v>
       </c>
-      <c r="E1134" s="104">
-        <v>600</v>
-      </c>
-      <c r="F1134" s="59"/>
-      <c r="G1134" s="15">
-        <v>1</v>
-      </c>
-      <c r="H1134" s="26"/>
-      <c r="I1134" s="107"/>
-      <c r="J1134" s="107"/>
-      <c r="K1134" s="27">
-        <v>605</v>
-      </c>
-      <c r="L1134" s="27">
+      <c r="L1133" s="27">
         <v>600</v>
       </c>
     </row>
@@ -42421,32 +42382,29 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="K4:L4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1135:C1048576 C1:C3">
-    <cfRule type="duplicateValues" dxfId="8" priority="25"/>
+  <conditionalFormatting sqref="C1134:C1048576 C1:C3">
+    <cfRule type="duplicateValues" dxfId="7" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C5">
-    <cfRule type="duplicateValues" dxfId="7" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C898 C962:C966">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C899:C960">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C961">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C967:C1021">
-    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1022:C1058">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1059:C1134">
-    <cfRule type="duplicateValues" dxfId="1" priority="27"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="C1059:C1133">
+    <cfRule type="duplicateValues" dxfId="0" priority="26"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -42479,14 +42437,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -42500,14 +42458,14 @@
       <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="133" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="134"/>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
+      <c r="A2" s="121" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -42549,10 +42507,10 @@
       <c r="C4" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="135" t="s">
+      <c r="D4" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="136"/>
+      <c r="E4" s="124"/>
       <c r="F4" s="36" t="s">
         <v>6</v>
       </c>
@@ -44590,10 +44548,10 @@
       <c r="C65" s="19" t="s">
         <v>948</v>
       </c>
-      <c r="D65" s="126">
+      <c r="D65" s="136">
         <v>690</v>
       </c>
-      <c r="E65" s="126">
+      <c r="E65" s="136">
         <v>680</v>
       </c>
       <c r="F65" s="15"/>
@@ -46579,7 +46537,7 @@
       </c>
       <c r="B124" s="2"/>
       <c r="C124" s="1" t="s">
-        <v>1733</v>
+        <v>1734</v>
       </c>
       <c r="D124" s="46">
         <v>640</v>
@@ -46608,7 +46566,7 @@
       </c>
       <c r="B125" s="2"/>
       <c r="C125" s="1" t="s">
-        <v>1734</v>
+        <v>1735</v>
       </c>
       <c r="D125" s="46">
         <v>615</v>
@@ -46637,7 +46595,7 @@
       </c>
       <c r="B126" s="2"/>
       <c r="C126" s="1" t="s">
-        <v>1735</v>
+        <v>1736</v>
       </c>
       <c r="D126" s="46">
         <v>560</v>
@@ -46666,7 +46624,7 @@
       </c>
       <c r="B127" s="2"/>
       <c r="C127" s="2" t="s">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="D127" s="46">
         <v>560</v>
@@ -46695,7 +46653,7 @@
       </c>
       <c r="B128" s="2"/>
       <c r="C128" s="2" t="s">
-        <v>1737</v>
+        <v>1738</v>
       </c>
       <c r="D128" s="46">
         <v>560</v>
@@ -46724,7 +46682,7 @@
       </c>
       <c r="B129" s="2"/>
       <c r="C129" s="2" t="s">
-        <v>1738</v>
+        <v>1739</v>
       </c>
       <c r="D129" s="46">
         <v>710</v>
@@ -46753,7 +46711,7 @@
       </c>
       <c r="B130" s="2"/>
       <c r="C130" s="2" t="s">
-        <v>1739</v>
+        <v>1740</v>
       </c>
       <c r="D130" s="46">
         <v>560</v>
@@ -46782,7 +46740,7 @@
       </c>
       <c r="B131" s="2"/>
       <c r="C131" s="2" t="s">
-        <v>1740</v>
+        <v>1741</v>
       </c>
       <c r="D131" s="46">
         <v>620</v>
@@ -46811,7 +46769,7 @@
       </c>
       <c r="B132" s="2"/>
       <c r="C132" s="2" t="s">
-        <v>1741</v>
+        <v>1742</v>
       </c>
       <c r="D132" s="46">
         <v>565</v>
@@ -46840,7 +46798,7 @@
       </c>
       <c r="B133" s="2"/>
       <c r="C133" s="2" t="s">
-        <v>1742</v>
+        <v>1743</v>
       </c>
       <c r="D133" s="46">
         <v>620</v>
@@ -46869,7 +46827,7 @@
       </c>
       <c r="B134" s="2"/>
       <c r="C134" s="2" t="s">
-        <v>1743</v>
+        <v>1744</v>
       </c>
       <c r="D134" s="46">
         <v>640</v>
@@ -46898,7 +46856,7 @@
       </c>
       <c r="B135" s="2"/>
       <c r="C135" s="2" t="s">
-        <v>1744</v>
+        <v>1745</v>
       </c>
       <c r="D135" s="46">
         <v>575</v>
@@ -46927,7 +46885,7 @@
       </c>
       <c r="B136" s="2"/>
       <c r="C136" s="2" t="s">
-        <v>1745</v>
+        <v>1746</v>
       </c>
       <c r="D136" s="46">
         <v>590</v>
@@ -46956,7 +46914,7 @@
       </c>
       <c r="B137" s="2"/>
       <c r="C137" s="2" t="s">
-        <v>1746</v>
+        <v>1747</v>
       </c>
       <c r="D137" s="46">
         <v>635</v>
@@ -46985,7 +46943,7 @@
       </c>
       <c r="B138" s="2"/>
       <c r="C138" s="2" t="s">
-        <v>1747</v>
+        <v>1748</v>
       </c>
       <c r="D138" s="46">
         <v>610</v>
@@ -47014,7 +46972,7 @@
       </c>
       <c r="B139" s="2"/>
       <c r="C139" s="2" t="s">
-        <v>1767</v>
+        <v>1768</v>
       </c>
       <c r="D139" s="46">
         <v>635</v>
@@ -47041,7 +46999,7 @@
       </c>
       <c r="B140" s="2"/>
       <c r="C140" s="2" t="s">
-        <v>1768</v>
+        <v>1769</v>
       </c>
       <c r="D140" s="46">
         <v>565</v>
@@ -47068,7 +47026,7 @@
       </c>
       <c r="B141" s="2"/>
       <c r="C141" s="2" t="s">
-        <v>1769</v>
+        <v>1770</v>
       </c>
       <c r="D141" s="46">
         <v>675</v>

</xml_diff>

<commit_message>
chore: update banners (2)
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F316768-91D4-2349-AAE4-265AAD283CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10161A1-C3CC-FC41-8EDB-F42CBBB81D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="1772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1834" uniqueCount="1773">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -5259,9 +5259,6 @@
     <t>Hoài Cảng LX</t>
   </si>
   <si>
-    <t>Vũ Jimmu</t>
-  </si>
-  <si>
     <t>Nguyễn Dũng</t>
   </si>
   <si>
@@ -5383,6 +5380,12 @@
   </si>
   <si>
     <t>0334113399</t>
+  </si>
+  <si>
+    <t>Nhàn Cấp Nước</t>
+  </si>
+  <si>
+    <t>Vũ Jimmy</t>
   </si>
 </sst>
 </file>
@@ -5998,32 +6001,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -6056,13 +6033,49 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bình thường 2" xfId="2" xr:uid="{2DBE829A-806A-A246-9A23-241A22DA22A4}"/>
     <cellStyle name="Bình thường 3" xfId="1" xr:uid="{ABA3F074-F600-1940-87D2-1B8571A799F2}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -7299,10 +7312,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L1133"/>
+  <dimension ref="A1:L1134"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1115" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K1128" sqref="K1128:L1133"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1107" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C1119" sqref="C1119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7322,30 +7335,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
       <c r="K1" s="25"/>
       <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="115" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
+      <c r="A2" s="127" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
       <c r="K2" s="25"/>
       <c r="L2" s="25"/>
     </row>
@@ -7371,10 +7384,10 @@
       <c r="C4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="117" t="s">
+      <c r="D4" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="118"/>
+      <c r="E4" s="130"/>
       <c r="F4" s="49" t="s">
         <v>6</v>
       </c>
@@ -7384,10 +7397,10 @@
       <c r="H4" s="31" t="s">
         <v>1415</v>
       </c>
-      <c r="K4" s="119" t="s">
+      <c r="K4" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="120"/>
+      <c r="L4" s="132"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="48"/>
@@ -10946,7 +10959,7 @@
         <v>585</v>
       </c>
       <c r="F117" s="81" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="G117" s="15">
         <v>1</v>
@@ -16875,7 +16888,7 @@
       </c>
       <c r="B305" s="51"/>
       <c r="C305" s="52" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="D305" s="75">
         <f t="shared" si="8"/>
@@ -17762,8 +17775,8 @@
         <v>329</v>
       </c>
       <c r="B334" s="51"/>
-      <c r="C334" s="128" t="s">
-        <v>1761</v>
+      <c r="C334" s="118" t="s">
+        <v>1760</v>
       </c>
       <c r="D334" s="75">
         <f t="shared" si="10"/>
@@ -34132,8 +34145,8 @@
         <v>856</v>
       </c>
       <c r="B861" s="53"/>
-      <c r="C861" s="135" t="s">
-        <v>1764</v>
+      <c r="C861" s="125" t="s">
+        <v>1763</v>
       </c>
       <c r="D861" s="75">
         <v>615</v>
@@ -37720,14 +37733,14 @@
         <v>972</v>
       </c>
       <c r="B977" s="1"/>
-      <c r="C977" s="126" t="s">
-        <v>1760</v>
-      </c>
-      <c r="D977" s="127">
+      <c r="C977" s="116" t="s">
+        <v>1759</v>
+      </c>
+      <c r="D977" s="117">
         <f t="shared" si="30"/>
         <v>610</v>
       </c>
-      <c r="E977" s="127">
+      <c r="E977" s="117">
         <f t="shared" si="31"/>
         <v>610</v>
       </c>
@@ -41848,7 +41861,7 @@
       </c>
       <c r="B1115" s="59"/>
       <c r="C1115" s="69" t="s">
-        <v>1730</v>
+        <v>1772</v>
       </c>
       <c r="D1115" s="75">
         <v>660</v>
@@ -41876,7 +41889,7 @@
       </c>
       <c r="B1116" s="59"/>
       <c r="C1116" s="69" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="D1116" s="75">
         <v>650</v>
@@ -41904,7 +41917,7 @@
       </c>
       <c r="B1117" s="59"/>
       <c r="C1117" s="69" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="D1117" s="75">
         <v>605</v>
@@ -41932,7 +41945,7 @@
       </c>
       <c r="B1118" s="59"/>
       <c r="C1118" s="69" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="D1118" s="75">
         <v>625</v>
@@ -41960,7 +41973,7 @@
       </c>
       <c r="B1119" s="59"/>
       <c r="C1119" s="69" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="D1119" s="75">
         <v>590</v>
@@ -41988,7 +42001,7 @@
       </c>
       <c r="B1120" s="59"/>
       <c r="C1120" s="69" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="D1120" s="75">
         <v>610</v>
@@ -42016,7 +42029,7 @@
       </c>
       <c r="B1121" s="59"/>
       <c r="C1121" s="69" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="D1121" s="75">
         <v>610</v>
@@ -42044,7 +42057,7 @@
       </c>
       <c r="B1122" s="59"/>
       <c r="C1122" s="69" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="D1122" s="75">
         <v>605</v>
@@ -42072,7 +42085,7 @@
       </c>
       <c r="B1123" s="59"/>
       <c r="C1123" s="69" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="D1123" s="75">
         <v>585</v>
@@ -42100,7 +42113,7 @@
       </c>
       <c r="B1124" s="59"/>
       <c r="C1124" s="69" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="D1124" s="75">
         <v>600</v>
@@ -42128,7 +42141,7 @@
       </c>
       <c r="B1125" s="59"/>
       <c r="C1125" s="69" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="D1125" s="75">
         <v>700</v>
@@ -42156,7 +42169,7 @@
       </c>
       <c r="B1126" s="59"/>
       <c r="C1126" s="69" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="D1126" s="75">
         <v>660</v>
@@ -42184,7 +42197,7 @@
       </c>
       <c r="B1127" s="59"/>
       <c r="C1127" s="69" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="D1127" s="75">
         <v>710</v>
@@ -42212,7 +42225,7 @@
       </c>
       <c r="B1128" s="59"/>
       <c r="C1128" s="69" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="D1128" s="75">
         <v>690</v>
@@ -42238,27 +42251,27 @@
       <c r="A1129" s="2">
         <v>1123</v>
       </c>
-      <c r="B1129" s="129"/>
-      <c r="C1129" s="130" t="s">
-        <v>1762</v>
-      </c>
-      <c r="D1129" s="131">
+      <c r="B1129" s="119"/>
+      <c r="C1129" s="120" t="s">
+        <v>1761</v>
+      </c>
+      <c r="D1129" s="121">
         <v>595</v>
       </c>
-      <c r="E1129" s="131">
+      <c r="E1129" s="121">
         <v>590</v>
       </c>
-      <c r="F1129" s="129"/>
+      <c r="F1129" s="119"/>
       <c r="G1129" s="15">
         <v>1</v>
       </c>
-      <c r="H1129" s="132"/>
-      <c r="I1129" s="133"/>
-      <c r="J1129" s="133"/>
-      <c r="K1129" s="134">
+      <c r="H1129" s="122"/>
+      <c r="I1129" s="123"/>
+      <c r="J1129" s="123"/>
+      <c r="K1129" s="124">
         <v>595</v>
       </c>
-      <c r="L1129" s="134">
+      <c r="L1129" s="124">
         <v>590</v>
       </c>
     </row>
@@ -42266,27 +42279,27 @@
       <c r="A1130" s="2">
         <v>1124</v>
       </c>
-      <c r="B1130" s="129"/>
-      <c r="C1130" s="130" t="s">
-        <v>1766</v>
-      </c>
-      <c r="D1130" s="131">
+      <c r="B1130" s="119"/>
+      <c r="C1130" s="120" t="s">
+        <v>1765</v>
+      </c>
+      <c r="D1130" s="121">
         <v>645</v>
       </c>
-      <c r="E1130" s="131">
+      <c r="E1130" s="121">
         <v>640</v>
       </c>
-      <c r="F1130" s="129"/>
+      <c r="F1130" s="119"/>
       <c r="G1130" s="15">
         <v>1</v>
       </c>
-      <c r="H1130" s="132"/>
-      <c r="I1130" s="133"/>
-      <c r="J1130" s="133"/>
-      <c r="K1130" s="134">
+      <c r="H1130" s="122"/>
+      <c r="I1130" s="123"/>
+      <c r="J1130" s="123"/>
+      <c r="K1130" s="124">
         <v>645</v>
       </c>
-      <c r="L1130" s="134">
+      <c r="L1130" s="124">
         <v>640</v>
       </c>
     </row>
@@ -42294,27 +42307,27 @@
       <c r="A1131" s="2">
         <v>1125</v>
       </c>
-      <c r="B1131" s="129"/>
-      <c r="C1131" s="130" t="s">
-        <v>1765</v>
-      </c>
-      <c r="D1131" s="131">
+      <c r="B1131" s="119"/>
+      <c r="C1131" s="120" t="s">
+        <v>1764</v>
+      </c>
+      <c r="D1131" s="121">
         <v>620</v>
       </c>
-      <c r="E1131" s="131">
+      <c r="E1131" s="121">
         <v>610</v>
       </c>
-      <c r="F1131" s="129"/>
+      <c r="F1131" s="119"/>
       <c r="G1131" s="15">
         <v>1</v>
       </c>
-      <c r="H1131" s="132"/>
-      <c r="I1131" s="133"/>
-      <c r="J1131" s="133"/>
-      <c r="K1131" s="134">
+      <c r="H1131" s="122"/>
+      <c r="I1131" s="123"/>
+      <c r="J1131" s="123"/>
+      <c r="K1131" s="124">
         <v>620</v>
       </c>
-      <c r="L1131" s="134">
+      <c r="L1131" s="124">
         <v>610</v>
       </c>
     </row>
@@ -42322,55 +42335,81 @@
       <c r="A1132" s="2">
         <v>1126</v>
       </c>
-      <c r="B1132" s="129"/>
-      <c r="C1132" s="130" t="s">
-        <v>1767</v>
-      </c>
-      <c r="D1132" s="131">
+      <c r="B1132" s="119"/>
+      <c r="C1132" s="120" t="s">
+        <v>1766</v>
+      </c>
+      <c r="D1132" s="121">
         <v>600</v>
       </c>
-      <c r="E1132" s="131">
+      <c r="E1132" s="121">
         <v>595</v>
       </c>
-      <c r="F1132" s="129"/>
+      <c r="F1132" s="119"/>
       <c r="G1132" s="15">
         <v>1</v>
       </c>
-      <c r="H1132" s="132"/>
-      <c r="I1132" s="133"/>
-      <c r="J1132" s="133"/>
-      <c r="K1132" s="134">
+      <c r="H1132" s="122"/>
+      <c r="I1132" s="123"/>
+      <c r="J1132" s="123"/>
+      <c r="K1132" s="124">
         <v>600</v>
       </c>
-      <c r="L1132" s="134">
+      <c r="L1132" s="124">
         <v>595</v>
       </c>
     </row>
     <row r="1133" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1133" s="114">
+      <c r="A1133" s="2">
+        <v>1267</v>
+      </c>
+      <c r="B1133" s="119"/>
+      <c r="C1133" s="120" t="s">
+        <v>1771</v>
+      </c>
+      <c r="D1133" s="121">
+        <v>645</v>
+      </c>
+      <c r="E1133" s="121"/>
+      <c r="F1133" s="119"/>
+      <c r="G1133" s="15">
+        <v>1</v>
+      </c>
+      <c r="H1133" s="122"/>
+      <c r="I1133" s="123"/>
+      <c r="J1133" s="123"/>
+      <c r="K1133" s="124">
+        <v>600</v>
+      </c>
+      <c r="L1133" s="124">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1134" s="114">
         <v>1136</v>
       </c>
-      <c r="B1133" s="59"/>
-      <c r="C1133" s="125" t="s">
-        <v>1759</v>
-      </c>
-      <c r="D1133" s="104">
+      <c r="B1134" s="59"/>
+      <c r="C1134" s="115" t="s">
+        <v>1758</v>
+      </c>
+      <c r="D1134" s="104">
         <v>605</v>
       </c>
-      <c r="E1133" s="104">
+      <c r="E1134" s="104">
         <v>600</v>
       </c>
-      <c r="F1133" s="59"/>
-      <c r="G1133" s="15">
-        <v>1</v>
-      </c>
-      <c r="H1133" s="26"/>
-      <c r="I1133" s="107"/>
-      <c r="J1133" s="107"/>
-      <c r="K1133" s="27">
+      <c r="F1134" s="59"/>
+      <c r="G1134" s="15">
+        <v>1</v>
+      </c>
+      <c r="H1134" s="26"/>
+      <c r="I1134" s="107"/>
+      <c r="J1134" s="107"/>
+      <c r="K1134" s="27">
         <v>605</v>
       </c>
-      <c r="L1133" s="27">
+      <c r="L1134" s="27">
         <v>600</v>
       </c>
     </row>
@@ -42382,29 +42421,32 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="K4:L4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1134:C1048576 C1:C3">
-    <cfRule type="duplicateValues" dxfId="7" priority="24"/>
+  <conditionalFormatting sqref="C1135:C1048576 C1:C3">
+    <cfRule type="duplicateValues" dxfId="8" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C5">
-    <cfRule type="duplicateValues" dxfId="6" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C898 C962:C966">
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C899:C960">
     <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C899:C960">
+  <conditionalFormatting sqref="C961">
     <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C961">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C967:C1021">
-    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1022:C1058">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1059:C1133">
-    <cfRule type="duplicateValues" dxfId="0" priority="26"/>
+  <conditionalFormatting sqref="C1059:C1134">
+    <cfRule type="duplicateValues" dxfId="1" priority="27"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -42437,14 +42479,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="133" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -42458,14 +42500,14 @@
       <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="121" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
+      <c r="A2" s="133" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="134"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -42507,10 +42549,10 @@
       <c r="C4" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="123" t="s">
+      <c r="D4" s="135" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="124"/>
+      <c r="E4" s="136"/>
       <c r="F4" s="36" t="s">
         <v>6</v>
       </c>
@@ -44548,10 +44590,10 @@
       <c r="C65" s="19" t="s">
         <v>948</v>
       </c>
-      <c r="D65" s="136">
+      <c r="D65" s="126">
         <v>690</v>
       </c>
-      <c r="E65" s="136">
+      <c r="E65" s="126">
         <v>680</v>
       </c>
       <c r="F65" s="15"/>
@@ -46537,7 +46579,7 @@
       </c>
       <c r="B124" s="2"/>
       <c r="C124" s="1" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="D124" s="46">
         <v>640</v>
@@ -46566,7 +46608,7 @@
       </c>
       <c r="B125" s="2"/>
       <c r="C125" s="1" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="D125" s="46">
         <v>615</v>
@@ -46595,7 +46637,7 @@
       </c>
       <c r="B126" s="2"/>
       <c r="C126" s="1" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="D126" s="46">
         <v>560</v>
@@ -46624,7 +46666,7 @@
       </c>
       <c r="B127" s="2"/>
       <c r="C127" s="2" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="D127" s="46">
         <v>560</v>
@@ -46653,7 +46695,7 @@
       </c>
       <c r="B128" s="2"/>
       <c r="C128" s="2" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="D128" s="46">
         <v>560</v>
@@ -46682,7 +46724,7 @@
       </c>
       <c r="B129" s="2"/>
       <c r="C129" s="2" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="D129" s="46">
         <v>710</v>
@@ -46711,7 +46753,7 @@
       </c>
       <c r="B130" s="2"/>
       <c r="C130" s="2" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="D130" s="46">
         <v>560</v>
@@ -46740,7 +46782,7 @@
       </c>
       <c r="B131" s="2"/>
       <c r="C131" s="2" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="D131" s="46">
         <v>620</v>
@@ -46769,7 +46811,7 @@
       </c>
       <c r="B132" s="2"/>
       <c r="C132" s="2" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="D132" s="46">
         <v>565</v>
@@ -46798,7 +46840,7 @@
       </c>
       <c r="B133" s="2"/>
       <c r="C133" s="2" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="D133" s="46">
         <v>620</v>
@@ -46827,7 +46869,7 @@
       </c>
       <c r="B134" s="2"/>
       <c r="C134" s="2" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="D134" s="46">
         <v>640</v>
@@ -46856,7 +46898,7 @@
       </c>
       <c r="B135" s="2"/>
       <c r="C135" s="2" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="D135" s="46">
         <v>575</v>
@@ -46885,7 +46927,7 @@
       </c>
       <c r="B136" s="2"/>
       <c r="C136" s="2" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="D136" s="46">
         <v>590</v>
@@ -46914,7 +46956,7 @@
       </c>
       <c r="B137" s="2"/>
       <c r="C137" s="2" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="D137" s="46">
         <v>635</v>
@@ -46943,7 +46985,7 @@
       </c>
       <c r="B138" s="2"/>
       <c r="C138" s="2" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="D138" s="46">
         <v>610</v>
@@ -46972,7 +47014,7 @@
       </c>
       <c r="B139" s="2"/>
       <c r="C139" s="2" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="D139" s="46">
         <v>635</v>
@@ -46999,7 +47041,7 @@
       </c>
       <c r="B140" s="2"/>
       <c r="C140" s="2" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="D140" s="46">
         <v>565</v>
@@ -47026,7 +47068,7 @@
       </c>
       <c r="B141" s="2"/>
       <c r="C141" s="2" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="D141" s="46">
         <v>675</v>

</xml_diff>

<commit_message>
chore: khanh da lat
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAA5553-DBFC-BB4B-AED4-A136B6E50F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583BB906-ED54-6249-993A-2EA10BFC504B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27260" yWindow="500" windowWidth="29080" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1871" uniqueCount="1806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="1807">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -5485,6 +5485,9 @@
   </si>
   <si>
     <t>Giải kỷ niệm btn</t>
+  </si>
+  <si>
+    <t>Anh Quốc</t>
   </si>
 </sst>
 </file>
@@ -7444,11 +7447,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P1161"/>
+  <dimension ref="A1:P1162"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A1081" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1102" sqref="C1:C1048576"/>
+      <pane ySplit="5" topLeftCell="A1151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1159" sqref="C1159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18398,11 +18401,11 @@
       </c>
       <c r="D308" s="47">
         <f t="shared" si="8"/>
-        <v>630</v>
+        <v>610</v>
       </c>
       <c r="E308" s="47">
         <f t="shared" si="9"/>
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="F308" s="50"/>
       <c r="G308" s="50">
@@ -18411,8 +18414,12 @@
       <c r="H308" s="14"/>
       <c r="I308" s="99"/>
       <c r="J308" s="99"/>
-      <c r="K308" s="79"/>
-      <c r="L308" s="79"/>
+      <c r="K308" s="79">
+        <v>-20</v>
+      </c>
+      <c r="L308" s="79">
+        <v>-20</v>
+      </c>
       <c r="M308" s="63"/>
       <c r="N308" s="63"/>
       <c r="O308" s="49">
@@ -48091,6 +48098,34 @@
       <c r="O1161" s="73"/>
       <c r="P1161" s="73"/>
     </row>
+    <row r="1162" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1162" s="2">
+        <v>1156</v>
+      </c>
+      <c r="B1162" s="69"/>
+      <c r="C1162" s="70" t="s">
+        <v>1806</v>
+      </c>
+      <c r="D1162" s="47">
+        <v>580</v>
+      </c>
+      <c r="E1162" s="47">
+        <v>580</v>
+      </c>
+      <c r="F1162" s="69"/>
+      <c r="G1162" s="50">
+        <v>1</v>
+      </c>
+      <c r="H1162" s="71"/>
+      <c r="I1162" s="104"/>
+      <c r="J1162" s="104"/>
+      <c r="K1162" s="83"/>
+      <c r="L1162" s="83"/>
+      <c r="M1162" s="72"/>
+      <c r="N1162" s="72"/>
+      <c r="O1162" s="73"/>
+      <c r="P1162" s="73"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0"/>
   <mergeCells count="4">
@@ -48099,7 +48134,7 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="O4:P4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1162:C1048576 C1:C3">
+  <conditionalFormatting sqref="C1163:C1048576 C1:C3">
     <cfRule type="duplicateValues" dxfId="9" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C5">
@@ -48123,7 +48158,7 @@
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1059:C1161">
+  <conditionalFormatting sqref="C1059:C1162">
     <cfRule type="duplicateValues" dxfId="1" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">

</xml_diff>

<commit_message>
chore: update nha can tho
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583BB906-ED54-6249-993A-2EA10BFC504B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7054569-5033-EB48-ACB0-F014DEE116DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7450,8 +7450,8 @@
   <dimension ref="A1:P1162"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A1151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1159" sqref="C1159"/>
+      <pane ySplit="5" topLeftCell="A921" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K932" sqref="A932:XFD932"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -40324,7 +40324,7 @@
       </c>
       <c r="D932" s="47">
         <f t="shared" si="28"/>
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="E932" s="47">
         <f t="shared" si="29"/>
@@ -40339,7 +40339,9 @@
       <c r="H932" s="13"/>
       <c r="I932" s="102"/>
       <c r="J932" s="102"/>
-      <c r="K932" s="79"/>
+      <c r="K932" s="79">
+        <v>-5</v>
+      </c>
       <c r="L932" s="79"/>
       <c r="M932" s="63">
         <v>5</v>

</xml_diff>

<commit_message>
chore: update score cao hoang thong
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812819FE-923E-1B49-83C0-21F7919892ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE943016-182C-AB40-BA11-5C1B9E9585F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6040,7 +6040,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -6298,6 +6298,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7565,8 +7568,8 @@
   <dimension ref="A1:P1208"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A1044" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1060" sqref="J1060"/>
+      <pane ySplit="5" topLeftCell="A563" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I574" sqref="I574"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -27980,7 +27983,7 @@
       </c>
       <c r="D574" s="45">
         <f t="shared" si="16"/>
-        <v>655</v>
+        <v>645</v>
       </c>
       <c r="E574" s="45">
         <f t="shared" si="17"/>
@@ -27993,7 +27996,9 @@
         <v>1</v>
       </c>
       <c r="H574" s="14"/>
-      <c r="I574" s="97"/>
+      <c r="I574" s="122">
+        <v>-10</v>
+      </c>
       <c r="J574" s="97"/>
       <c r="K574" s="77"/>
       <c r="L574" s="77"/>

</xml_diff>

<commit_message>
chore: update quy mpd
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE943016-182C-AB40-BA11-5C1B9E9585F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FF734B-BD75-114E-8C38-ED79CBD7F710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="1850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1920" uniqueCount="1851">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -5620,6 +5620,9 @@
   </si>
   <si>
     <t>win79</t>
+  </si>
+  <si>
+    <t>Viết Hòa</t>
   </si>
 </sst>
 </file>
@@ -6275,6 +6278,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6298,9 +6304,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7565,11 +7568,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P1208"/>
+  <dimension ref="A1:P1209"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A563" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I574" sqref="I574"/>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A1177" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7592,30 +7595,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:16" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
+      <c r="A2" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
       <c r="I2" s="30"/>
       <c r="J2" s="30"/>
     </row>
@@ -7643,10 +7646,10 @@
       <c r="C4" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="116" t="s">
+      <c r="D4" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="117"/>
+      <c r="E4" s="118"/>
       <c r="F4" s="106" t="s">
         <v>6</v>
       </c>
@@ -7666,10 +7669,10 @@
       <c r="M4" s="111" t="s">
         <v>1805</v>
       </c>
-      <c r="O4" s="116" t="s">
+      <c r="O4" s="117" t="s">
         <v>1804</v>
       </c>
-      <c r="P4" s="117"/>
+      <c r="P4" s="118"/>
     </row>
     <row r="5" spans="1:16" s="105" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="99"/>
@@ -11439,7 +11442,7 @@
       </c>
       <c r="E108" s="45">
         <f t="shared" si="3"/>
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="F108" s="46" t="s">
         <v>122</v>
@@ -11449,7 +11452,9 @@
       </c>
       <c r="H108" s="14"/>
       <c r="I108" s="97"/>
-      <c r="J108" s="97"/>
+      <c r="J108" s="97">
+        <v>-5</v>
+      </c>
       <c r="K108" s="77"/>
       <c r="L108" s="77"/>
       <c r="M108" s="61">
@@ -27983,7 +27988,7 @@
       </c>
       <c r="D574" s="45">
         <f t="shared" si="16"/>
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="E574" s="45">
         <f t="shared" si="17"/>
@@ -27996,8 +28001,8 @@
         <v>1</v>
       </c>
       <c r="H574" s="14"/>
-      <c r="I574" s="122">
-        <v>-10</v>
+      <c r="I574" s="112">
+        <v>-15</v>
       </c>
       <c r="J574" s="97"/>
       <c r="K574" s="77"/>
@@ -49505,7 +49510,7 @@
       </c>
       <c r="E1188" s="45">
         <f t="shared" si="37"/>
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="F1188" s="67"/>
       <c r="G1188" s="48">
@@ -49516,7 +49521,7 @@
         <v>-5</v>
       </c>
       <c r="J1188" s="97">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="K1188" s="81"/>
       <c r="L1188" s="81"/>
@@ -50223,6 +50228,40 @@
       </c>
       <c r="P1208" s="71">
         <v>600</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1209" s="1">
+        <v>1204</v>
+      </c>
+      <c r="B1209" s="67"/>
+      <c r="C1209" s="68" t="s">
+        <v>1850</v>
+      </c>
+      <c r="D1209" s="45">
+        <f t="shared" ref="D1209" si="40">O1209+M1209+K1209+I1209</f>
+        <v>590</v>
+      </c>
+      <c r="E1209" s="45">
+        <f t="shared" ref="E1209" si="41">N1209+P1209+L1209+J1209</f>
+        <v>585</v>
+      </c>
+      <c r="F1209" s="67"/>
+      <c r="G1209" s="48">
+        <v>1</v>
+      </c>
+      <c r="H1209" s="69"/>
+      <c r="I1209" s="97"/>
+      <c r="J1209" s="97"/>
+      <c r="K1209" s="81"/>
+      <c r="L1209" s="81"/>
+      <c r="M1209" s="70"/>
+      <c r="N1209" s="70"/>
+      <c r="O1209" s="71">
+        <v>590</v>
+      </c>
+      <c r="P1209" s="71">
+        <v>585</v>
       </c>
     </row>
   </sheetData>
@@ -50236,7 +50275,7 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="O4:P4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1209:C1048576 C1:C3">
+  <conditionalFormatting sqref="C1210:C1048576 C1:C3">
     <cfRule type="duplicateValues" dxfId="9" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C5">
@@ -50260,7 +50299,7 @@
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1059:C1208">
+  <conditionalFormatting sqref="C1059:C1209">
     <cfRule type="duplicateValues" dxfId="1" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
@@ -50273,7 +50312,7 @@
   </headerFooter>
   <ignoredErrors>
     <ignoredError sqref="E6:E1207 D6:D1207" unlockedFormula="1"/>
-    <ignoredError sqref="F6:F1304" numberStoredAsText="1"/>
+    <ignoredError sqref="F6:F1208 F1210:F1304" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -50283,9 +50322,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A144" sqref="A144:XFD144"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -50301,14 +50340,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
       <c r="G1" s="73"/>
       <c r="H1" s="73"/>
       <c r="I1" s="73"/>
@@ -50322,14 +50361,14 @@
       <c r="Q1" s="73"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="118" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
+      <c r="A2" s="119" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
       <c r="G2" s="73"/>
       <c r="H2" s="73"/>
       <c r="I2" s="73"/>
@@ -50371,10 +50410,10 @@
       <c r="C4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="120" t="s">
+      <c r="D4" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="121"/>
+      <c r="E4" s="122"/>
       <c r="F4" s="74" t="s">
         <v>6</v>
       </c>
@@ -52586,10 +52625,10 @@
         <v>957</v>
       </c>
       <c r="D70" s="85">
-        <v>615</v>
+        <v>605</v>
       </c>
       <c r="E70" s="85">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="F70" s="46" t="s">
         <v>958</v>

</xml_diff>

<commit_message>
chore: nhan cap nuoc 640
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FF734B-BD75-114E-8C38-ED79CBD7F710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59320884-7B84-2946-A577-4120863E7BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -7570,9 +7570,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P1209"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A1177" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C1:C1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A1122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J1134" sqref="J1134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14354,11 +14354,11 @@
       </c>
       <c r="D190" s="45">
         <f t="shared" si="4"/>
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="E190" s="45">
         <f t="shared" si="5"/>
-        <v>670</v>
+        <v>655</v>
       </c>
       <c r="F190" s="48"/>
       <c r="G190" s="48">
@@ -14366,10 +14366,10 @@
       </c>
       <c r="H190" s="14"/>
       <c r="I190" s="97">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="J190" s="97">
-        <v>-5</v>
+        <v>-20</v>
       </c>
       <c r="K190" s="77">
         <v>-5</v>
@@ -47600,11 +47600,11 @@
       </c>
       <c r="D1133" s="45">
         <f t="shared" si="34"/>
-        <v>595</v>
+        <v>640</v>
       </c>
       <c r="E1133" s="45">
         <f t="shared" si="35"/>
-        <v>590</v>
+        <v>630</v>
       </c>
       <c r="F1133" s="67"/>
       <c r="G1133" s="48">
@@ -47612,10 +47612,10 @@
       </c>
       <c r="H1133" s="69"/>
       <c r="I1133" s="97">
-        <v>-5</v>
+        <v>40</v>
       </c>
       <c r="J1133" s="97">
-        <v>-5</v>
+        <v>35</v>
       </c>
       <c r="K1133" s="81"/>
       <c r="L1133" s="81"/>
@@ -47816,7 +47816,7 @@
       </c>
       <c r="D1139" s="45">
         <f t="shared" si="34"/>
-        <v>670</v>
+        <v>640</v>
       </c>
       <c r="E1139" s="45">
         <f t="shared" si="35"/>
@@ -47827,7 +47827,9 @@
         <v>1</v>
       </c>
       <c r="H1139" s="69"/>
-      <c r="I1139" s="97"/>
+      <c r="I1139" s="97">
+        <v>-30</v>
+      </c>
       <c r="J1139" s="97"/>
       <c r="K1139" s="81">
         <v>30</v>
@@ -50322,9 +50324,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
chore: update dung hd
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59320884-7B84-2946-A577-4120863E7BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C0941E-4388-1C4B-BC0E-17C5BE9B6D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7571,8 +7571,8 @@
   <dimension ref="A1:P1209"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A1122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1134" sqref="J1134"/>
+      <pane ySplit="5" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K117" sqref="K117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11762,11 +11762,11 @@
       </c>
       <c r="D117" s="45">
         <f t="shared" si="2"/>
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="E117" s="45">
         <f t="shared" si="3"/>
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="F117" s="50" t="s">
         <v>1769</v>
@@ -11775,8 +11775,12 @@
         <v>1</v>
       </c>
       <c r="H117" s="14"/>
-      <c r="I117" s="97"/>
-      <c r="J117" s="97"/>
+      <c r="I117" s="97">
+        <v>-5</v>
+      </c>
+      <c r="J117" s="97">
+        <v>-5</v>
+      </c>
       <c r="K117" s="77"/>
       <c r="L117" s="77"/>
       <c r="M117" s="61"/>

</xml_diff>

<commit_message>
chore: viet ton 590
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C0941E-4388-1C4B-BC0E-17C5BE9B6D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A205DAC-EA67-EF45-9CCA-674E667A19F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7571,8 +7571,8 @@
   <dimension ref="A1:P1209"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K117" sqref="K117"/>
+      <pane ySplit="5" topLeftCell="A1042" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1053" sqref="K1053"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -44814,19 +44814,23 @@
       </c>
       <c r="D1053" s="45">
         <f t="shared" si="32"/>
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="E1053" s="45">
         <f t="shared" si="33"/>
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="F1053" s="59"/>
       <c r="G1053" s="48">
         <v>1</v>
       </c>
       <c r="H1053" s="17"/>
-      <c r="I1053" s="97"/>
-      <c r="J1053" s="97"/>
+      <c r="I1053" s="97">
+        <v>-5</v>
+      </c>
+      <c r="J1053" s="97">
+        <v>-5</v>
+      </c>
       <c r="K1053" s="77"/>
       <c r="L1053" s="77"/>
       <c r="M1053" s="61"/>

</xml_diff>

<commit_message>
chore: min 580 for all
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A205DAC-EA67-EF45-9CCA-674E667A19F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237B96AE-DAF7-B44B-9487-93016C41DCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7571,8 +7571,8 @@
   <dimension ref="A1:P1209"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A1042" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1053" sqref="K1053"/>
+      <pane ySplit="5" topLeftCell="A975" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J987" sqref="J987"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26088,7 +26088,7 @@
       </c>
       <c r="E520" s="45">
         <f t="shared" si="17"/>
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="F520" s="46" t="s">
         <v>665</v>
@@ -26101,7 +26101,7 @@
         <v>-5</v>
       </c>
       <c r="J520" s="97">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="K520" s="77"/>
       <c r="L520" s="77"/>
@@ -42512,7 +42512,7 @@
       </c>
       <c r="E986" s="45">
         <f t="shared" si="31"/>
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="F986" s="48"/>
       <c r="G986" s="48">
@@ -42523,7 +42523,7 @@
         <v>-5</v>
       </c>
       <c r="J986" s="97">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="K986" s="77"/>
       <c r="L986" s="77"/>
@@ -48780,11 +48780,11 @@
       </c>
       <c r="D1167" s="45">
         <f t="shared" si="36"/>
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="E1167" s="45">
         <f t="shared" si="37"/>
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="F1167" s="67"/>
       <c r="G1167" s="48">
@@ -48792,10 +48792,10 @@
       </c>
       <c r="H1167" s="69"/>
       <c r="I1167" s="97">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="J1167" s="97">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="K1167" s="81"/>
       <c r="L1167" s="81"/>

</xml_diff>

<commit_message>
chore: update score quoc dat
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B38D91A-ED96-B744-851E-8765BC922127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273BC475-4D79-CC46-832E-AF9977FF3971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29040" yWindow="500" windowWidth="19740" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -7889,8 +7889,8 @@
   <dimension ref="A1:R1237"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q65" sqref="Q65"/>
+      <pane ySplit="5" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J112" sqref="J112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12129,7 +12129,7 @@
       </c>
       <c r="E111" s="44">
         <f t="shared" si="9"/>
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="F111" s="47"/>
       <c r="G111" s="47">
@@ -12137,7 +12137,9 @@
       </c>
       <c r="H111" s="14"/>
       <c r="I111" s="112"/>
-      <c r="J111" s="112"/>
+      <c r="J111" s="112">
+        <v>-5</v>
+      </c>
       <c r="K111" s="96"/>
       <c r="L111" s="96"/>
       <c r="M111" s="76"/>
@@ -39990,7 +39992,7 @@
       </c>
       <c r="E855" s="44">
         <f t="shared" si="47"/>
-        <v>615</v>
+        <v>605</v>
       </c>
       <c r="F855" s="47" t="s">
         <v>1407</v>
@@ -40000,7 +40002,9 @@
       </c>
       <c r="H855" s="14"/>
       <c r="I855" s="112"/>
-      <c r="J855" s="112"/>
+      <c r="J855" s="112">
+        <v>-10</v>
+      </c>
       <c r="K855" s="96"/>
       <c r="L855" s="96"/>
       <c r="M855" s="76"/>
@@ -49156,19 +49160,23 @@
       </c>
       <c r="D1102" s="44">
         <f t="shared" si="54"/>
-        <v>665</v>
+        <v>620</v>
       </c>
       <c r="E1102" s="44">
         <f t="shared" si="55"/>
-        <v>635</v>
+        <v>620</v>
       </c>
       <c r="F1102" s="34"/>
       <c r="G1102" s="47">
         <v>1</v>
       </c>
       <c r="H1102" s="17"/>
-      <c r="I1102" s="119"/>
-      <c r="J1102" s="119"/>
+      <c r="I1102" s="119">
+        <v>-45</v>
+      </c>
+      <c r="J1102" s="119">
+        <v>-15</v>
+      </c>
       <c r="K1102" s="96">
         <v>-5</v>
       </c>

</xml_diff>

<commit_message>
chore: update hoai canada
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273BC475-4D79-CC46-832E-AF9977FF3971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86572C12-9471-2E4C-B0A9-82317D6BC69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27700" yWindow="2660" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -7890,7 +7890,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J112" sqref="J112"/>
+      <selection pane="bottomLeft" activeCell="I103" sqref="I103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11775,7 +11775,7 @@
       </c>
       <c r="D102" s="44">
         <f t="shared" si="8"/>
-        <v>590</v>
+        <v>580</v>
       </c>
       <c r="E102" s="44">
         <f t="shared" si="9"/>
@@ -11786,7 +11786,9 @@
         <v>1</v>
       </c>
       <c r="H102" s="14"/>
-      <c r="I102" s="112"/>
+      <c r="I102" s="112">
+        <v>-10</v>
+      </c>
       <c r="J102" s="112"/>
       <c r="K102" s="96"/>
       <c r="L102" s="96"/>

</xml_diff>

<commit_message>
chore: del duong hoang nhat
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86572C12-9471-2E4C-B0A9-82317D6BC69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E8AD74-6595-D746-AD16-3618406293BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27700" yWindow="2660" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1971" uniqueCount="1897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1971" uniqueCount="1896">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -5336,9 +5336,6 @@
   </si>
   <si>
     <t>Duy Em</t>
-  </si>
-  <si>
-    <t>Dương - Hoàng Nhật</t>
   </si>
   <si>
     <t>Trường An Nhơn</t>
@@ -7889,8 +7886,8 @@
   <dimension ref="A1:R1237"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I103" sqref="I103"/>
+      <pane ySplit="5" topLeftCell="A850" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I861" sqref="I861"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7979,27 +7976,27 @@
         <v>6</v>
       </c>
       <c r="G4" s="105" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="H4" s="106" t="s">
         <v>1412</v>
       </c>
       <c r="I4" s="120" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="J4" s="106"/>
       <c r="K4" s="106" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="L4" s="106"/>
       <c r="M4" s="110" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="O4" s="110" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="Q4" s="141" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="R4" s="142"/>
     </row>
@@ -11219,7 +11216,7 @@
       </c>
       <c r="H87" s="15"/>
       <c r="I87" s="114" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="J87" s="114"/>
       <c r="K87" s="96"/>
@@ -12364,7 +12361,7 @@
         <v>580</v>
       </c>
       <c r="F117" s="49" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="G117" s="47">
         <v>1</v>
@@ -13350,7 +13347,7 @@
       </c>
       <c r="B143" s="27"/>
       <c r="C143" s="28" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="D143" s="44">
         <f t="shared" si="8"/>
@@ -19268,7 +19265,7 @@
       </c>
       <c r="B300" s="27"/>
       <c r="C300" s="28" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="D300" s="44">
         <f t="shared" si="22"/>
@@ -39502,7 +39499,7 @@
       </c>
       <c r="B842" s="29"/>
       <c r="C842" s="37" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="D842" s="44">
         <f t="shared" si="46"/>
@@ -40212,21 +40209,19 @@
       </c>
       <c r="B861" s="29"/>
       <c r="C861" s="71" t="s">
-        <v>1755</v>
+        <v>1162</v>
       </c>
       <c r="D861" s="44">
-        <f t="shared" si="46"/>
-        <v>630</v>
+        <v>0</v>
       </c>
       <c r="E861" s="44">
-        <f t="shared" si="47"/>
-        <v>615</v>
+        <v>0</v>
       </c>
       <c r="F861" s="47" t="s">
         <v>1410</v>
       </c>
       <c r="G861" s="47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H861" s="14"/>
       <c r="I861" s="112"/>
@@ -49640,7 +49635,7 @@
       </c>
       <c r="B1115" s="34"/>
       <c r="C1115" s="43" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="D1115" s="44">
         <f t="shared" si="54"/>
@@ -49792,7 +49787,7 @@
       </c>
       <c r="B1119" s="34"/>
       <c r="C1119" s="43" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="D1119" s="44">
         <f t="shared" si="54"/>
@@ -50190,7 +50185,7 @@
       </c>
       <c r="B1130" s="66"/>
       <c r="C1130" s="67" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="D1130" s="44">
         <f t="shared" si="56"/>
@@ -50230,7 +50225,7 @@
       </c>
       <c r="B1131" s="66"/>
       <c r="C1131" s="67" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="D1131" s="44">
         <f t="shared" si="56"/>
@@ -50266,7 +50261,7 @@
       </c>
       <c r="B1132" s="66"/>
       <c r="C1132" s="67" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="D1132" s="44">
         <f t="shared" si="56"/>
@@ -50302,7 +50297,7 @@
       </c>
       <c r="B1133" s="66"/>
       <c r="C1133" s="67" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="D1133" s="44">
         <f t="shared" si="56"/>
@@ -50344,7 +50339,7 @@
       </c>
       <c r="B1134" s="66"/>
       <c r="C1134" s="67" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="D1134" s="44">
         <f t="shared" si="56"/>
@@ -50380,7 +50375,7 @@
       </c>
       <c r="B1135" s="66"/>
       <c r="C1135" s="67" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="D1135" s="44">
         <f t="shared" si="56"/>
@@ -50420,7 +50415,7 @@
       </c>
       <c r="B1136" s="66"/>
       <c r="C1136" s="67" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="D1136" s="44">
         <f t="shared" si="56"/>
@@ -50456,7 +50451,7 @@
       </c>
       <c r="B1137" s="66"/>
       <c r="C1137" s="67" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="D1137" s="44">
         <f t="shared" si="56"/>
@@ -50492,7 +50487,7 @@
       </c>
       <c r="B1138" s="66"/>
       <c r="C1138" s="67" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="D1138" s="44">
         <f t="shared" si="56"/>
@@ -50537,7 +50532,7 @@
       </c>
       <c r="B1139" s="66"/>
       <c r="C1139" s="67" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D1139" s="44">
         <f t="shared" si="56"/>
@@ -50579,7 +50574,7 @@
       </c>
       <c r="B1140" s="66"/>
       <c r="C1140" s="67" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D1140" s="44">
         <f t="shared" si="56"/>
@@ -50615,7 +50610,7 @@
       </c>
       <c r="B1141" s="66"/>
       <c r="C1141" s="67" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="D1141" s="44">
         <f t="shared" si="56"/>
@@ -50651,7 +50646,7 @@
       </c>
       <c r="B1142" s="66"/>
       <c r="C1142" s="67" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="D1142" s="44">
         <f t="shared" si="56"/>
@@ -50689,7 +50684,7 @@
       </c>
       <c r="B1143" s="66"/>
       <c r="C1143" s="67" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="D1143" s="44">
         <f t="shared" si="56"/>
@@ -50725,7 +50720,7 @@
       </c>
       <c r="B1144" s="66"/>
       <c r="C1144" s="67" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="D1144" s="44">
         <f t="shared" si="56"/>
@@ -50761,7 +50756,7 @@
       </c>
       <c r="B1145" s="66"/>
       <c r="C1145" s="67" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="D1145" s="44">
         <f t="shared" si="56"/>
@@ -50797,7 +50792,7 @@
       </c>
       <c r="B1146" s="66"/>
       <c r="C1146" s="67" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="D1146" s="44">
         <f t="shared" si="56"/>
@@ -50833,7 +50828,7 @@
       </c>
       <c r="B1147" s="66"/>
       <c r="C1147" s="67" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="D1147" s="44">
         <f t="shared" si="56"/>
@@ -50869,7 +50864,7 @@
       </c>
       <c r="B1148" s="66"/>
       <c r="C1148" s="67" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="D1148" s="44">
         <f t="shared" si="56"/>
@@ -50905,7 +50900,7 @@
       </c>
       <c r="B1149" s="66"/>
       <c r="C1149" s="67" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="D1149" s="44">
         <f t="shared" si="56"/>
@@ -50977,7 +50972,7 @@
       </c>
       <c r="B1151" s="66"/>
       <c r="C1151" s="67" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="D1151" s="44">
         <f t="shared" ref="D1151:D1164" si="60">Q1151+O1151+M1151+K1151+I1151</f>
@@ -51013,7 +51008,7 @@
       </c>
       <c r="B1152" s="66"/>
       <c r="C1152" s="67" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="D1152" s="44">
         <f t="shared" si="60"/>
@@ -51049,7 +51044,7 @@
       </c>
       <c r="B1153" s="66"/>
       <c r="C1153" s="67" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="D1153" s="44">
         <f t="shared" si="60"/>
@@ -51085,7 +51080,7 @@
       </c>
       <c r="B1154" s="66"/>
       <c r="C1154" s="67" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="D1154" s="44">
         <f t="shared" si="60"/>
@@ -51121,7 +51116,7 @@
       </c>
       <c r="B1155" s="66"/>
       <c r="C1155" s="67" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="D1155" s="44">
         <f t="shared" si="60"/>
@@ -51157,7 +51152,7 @@
       </c>
       <c r="B1156" s="66"/>
       <c r="C1156" s="67" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="D1156" s="44">
         <f t="shared" si="60"/>
@@ -51193,7 +51188,7 @@
       </c>
       <c r="B1157" s="66"/>
       <c r="C1157" s="67" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="D1157" s="44">
         <f t="shared" si="60"/>
@@ -51229,7 +51224,7 @@
       </c>
       <c r="B1158" s="66"/>
       <c r="C1158" s="67" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="D1158" s="44">
         <f t="shared" si="60"/>
@@ -51265,7 +51260,7 @@
       </c>
       <c r="B1159" s="66"/>
       <c r="C1159" s="67" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="D1159" s="44">
         <f t="shared" si="60"/>
@@ -51301,7 +51296,7 @@
       </c>
       <c r="B1160" s="66"/>
       <c r="C1160" s="67" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="D1160" s="44">
         <f t="shared" si="60"/>
@@ -51337,7 +51332,7 @@
       </c>
       <c r="B1161" s="66"/>
       <c r="C1161" s="67" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="D1161" s="44">
         <f t="shared" si="60"/>
@@ -51407,7 +51402,7 @@
       </c>
       <c r="B1163" s="66"/>
       <c r="C1163" s="67" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="D1163" s="44">
         <f t="shared" si="60"/>
@@ -51443,7 +51438,7 @@
       </c>
       <c r="B1164" s="66"/>
       <c r="C1164" s="67" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="D1164" s="44">
         <f t="shared" si="60"/>
@@ -51517,7 +51512,7 @@
       </c>
       <c r="B1166" s="66"/>
       <c r="C1166" s="67" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="D1166" s="44">
         <f t="shared" ref="D1166:D1190" si="62">Q1166+O1166+M1166+K1166+I1166</f>
@@ -51553,7 +51548,7 @@
       </c>
       <c r="B1167" s="66"/>
       <c r="C1167" s="67" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="D1167" s="44">
         <f t="shared" si="62"/>
@@ -51593,7 +51588,7 @@
       </c>
       <c r="B1168" s="66"/>
       <c r="C1168" s="67" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="D1168" s="44">
         <f t="shared" si="62"/>
@@ -51629,7 +51624,7 @@
       </c>
       <c r="B1169" s="66"/>
       <c r="C1169" s="67" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="D1169" s="44">
         <f t="shared" si="62"/>
@@ -51663,7 +51658,7 @@
       </c>
       <c r="B1170" s="66"/>
       <c r="C1170" s="67" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="D1170" s="44">
         <f t="shared" si="62"/>
@@ -51703,7 +51698,7 @@
       </c>
       <c r="B1171" s="66"/>
       <c r="C1171" s="67" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="D1171" s="44">
         <f t="shared" si="62"/>
@@ -51743,7 +51738,7 @@
       </c>
       <c r="B1172" s="66"/>
       <c r="C1172" s="67" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="D1172" s="44">
         <f t="shared" si="62"/>
@@ -51779,7 +51774,7 @@
       </c>
       <c r="B1173" s="66"/>
       <c r="C1173" s="67" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="D1173" s="44">
         <f t="shared" si="62"/>
@@ -51815,7 +51810,7 @@
       </c>
       <c r="B1174" s="66"/>
       <c r="C1174" s="67" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="D1174" s="44">
         <f t="shared" si="62"/>
@@ -51851,7 +51846,7 @@
       </c>
       <c r="B1175" s="66"/>
       <c r="C1175" s="67" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="D1175" s="44">
         <f t="shared" si="62"/>
@@ -51923,7 +51918,7 @@
       </c>
       <c r="B1177" s="66"/>
       <c r="C1177" s="67" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="D1177" s="44">
         <f t="shared" si="62"/>
@@ -51961,7 +51956,7 @@
       </c>
       <c r="B1178" s="66"/>
       <c r="C1178" s="67" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="D1178" s="44">
         <f t="shared" si="62"/>
@@ -51997,7 +51992,7 @@
       </c>
       <c r="B1179" s="66"/>
       <c r="C1179" s="67" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="D1179" s="44">
         <f t="shared" si="62"/>
@@ -52033,7 +52028,7 @@
       </c>
       <c r="B1180" s="66"/>
       <c r="C1180" s="67" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="D1180" s="44">
         <f t="shared" si="62"/>
@@ -52069,7 +52064,7 @@
       </c>
       <c r="B1181" s="66"/>
       <c r="C1181" s="67" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="D1181" s="44">
         <f t="shared" si="62"/>
@@ -52109,7 +52104,7 @@
       </c>
       <c r="B1182" s="66"/>
       <c r="C1182" s="67" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="D1182" s="44">
         <f t="shared" si="62"/>
@@ -52149,7 +52144,7 @@
       </c>
       <c r="B1183" s="66"/>
       <c r="C1183" s="67" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="D1183" s="44">
         <f t="shared" si="62"/>
@@ -52189,7 +52184,7 @@
       </c>
       <c r="B1184" s="66"/>
       <c r="C1184" s="67" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="D1184" s="44">
         <f t="shared" si="62"/>
@@ -52225,7 +52220,7 @@
       </c>
       <c r="B1185" s="66"/>
       <c r="C1185" s="67" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="D1185" s="44">
         <f t="shared" si="62"/>
@@ -52261,7 +52256,7 @@
       </c>
       <c r="B1186" s="66"/>
       <c r="C1186" s="67" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="D1186" s="44">
         <f t="shared" si="62"/>
@@ -52299,7 +52294,7 @@
       </c>
       <c r="B1187" s="66"/>
       <c r="C1187" s="67" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="D1187" s="44">
         <f t="shared" si="62"/>
@@ -52335,7 +52330,7 @@
       </c>
       <c r="B1188" s="66"/>
       <c r="C1188" s="67" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="D1188" s="44">
         <f t="shared" si="62"/>
@@ -52375,7 +52370,7 @@
       </c>
       <c r="B1189" s="66"/>
       <c r="C1189" s="67" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="D1189" s="44">
         <f t="shared" si="62"/>
@@ -52415,7 +52410,7 @@
       </c>
       <c r="B1190" s="66"/>
       <c r="C1190" s="67" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="D1190" s="44">
         <f t="shared" si="62"/>
@@ -52451,7 +52446,7 @@
       </c>
       <c r="B1191" s="66"/>
       <c r="C1191" s="67" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="D1191" s="44">
         <f>Q1191+O1191+M1191+K1191</f>
@@ -52521,7 +52516,7 @@
       </c>
       <c r="B1193" s="66"/>
       <c r="C1193" s="67" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="D1193" s="44">
         <f t="shared" ref="D1193:D1208" si="64">Q1193+O1193+M1193+K1193+I1193</f>
@@ -52557,7 +52552,7 @@
       </c>
       <c r="B1194" s="66"/>
       <c r="C1194" s="67" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="D1194" s="44">
         <f t="shared" si="64"/>
@@ -52593,7 +52588,7 @@
       </c>
       <c r="B1195" s="66"/>
       <c r="C1195" s="67" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="D1195" s="44">
         <f t="shared" si="64"/>
@@ -52633,7 +52628,7 @@
       </c>
       <c r="B1196" s="66"/>
       <c r="C1196" s="67" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="D1196" s="44">
         <f t="shared" si="64"/>
@@ -52673,7 +52668,7 @@
       </c>
       <c r="B1197" s="66"/>
       <c r="C1197" s="67" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="D1197" s="44">
         <f t="shared" si="64"/>
@@ -52709,7 +52704,7 @@
       </c>
       <c r="B1198" s="66"/>
       <c r="C1198" s="67" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="D1198" s="44">
         <f t="shared" si="64"/>
@@ -52745,7 +52740,7 @@
       </c>
       <c r="B1199" s="66"/>
       <c r="C1199" s="67" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="D1199" s="44">
         <f t="shared" si="64"/>
@@ -52781,7 +52776,7 @@
       </c>
       <c r="B1200" s="66"/>
       <c r="C1200" s="67" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="D1200" s="44">
         <f t="shared" si="64"/>
@@ -52819,7 +52814,7 @@
       </c>
       <c r="B1201" s="66"/>
       <c r="C1201" s="67" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="D1201" s="44">
         <f t="shared" si="64"/>
@@ -52855,7 +52850,7 @@
       </c>
       <c r="B1202" s="66"/>
       <c r="C1202" s="67" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D1202" s="44">
         <f t="shared" si="64"/>
@@ -52891,7 +52886,7 @@
       </c>
       <c r="B1203" s="66"/>
       <c r="C1203" s="67" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="D1203" s="44">
         <f t="shared" si="64"/>
@@ -52931,7 +52926,7 @@
       </c>
       <c r="B1204" s="66"/>
       <c r="C1204" s="67" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="D1204" s="44">
         <f t="shared" si="64"/>
@@ -53001,7 +52996,7 @@
       </c>
       <c r="B1206" s="66"/>
       <c r="C1206" s="67" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="D1206" s="44">
         <f t="shared" si="64"/>
@@ -53037,7 +53032,7 @@
       </c>
       <c r="B1207" s="66"/>
       <c r="C1207" s="67" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="D1207" s="44">
         <f t="shared" si="64"/>
@@ -53073,7 +53068,7 @@
       </c>
       <c r="B1208" s="66"/>
       <c r="C1208" s="67" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="D1208" s="44">
         <f t="shared" si="64"/>
@@ -53109,7 +53104,7 @@
       </c>
       <c r="B1209" s="66"/>
       <c r="C1209" s="67" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="D1209" s="44">
         <f t="shared" ref="D1209:D1221" si="66">Q1209+O1209+M1209+K1209+I1209</f>
@@ -53145,7 +53140,7 @@
       </c>
       <c r="B1210" s="66"/>
       <c r="C1210" s="67" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="D1210" s="44">
         <f t="shared" si="66"/>
@@ -53181,7 +53176,7 @@
       </c>
       <c r="B1211" s="66"/>
       <c r="C1211" s="67" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="D1211" s="44">
         <f t="shared" si="66"/>
@@ -53219,7 +53214,7 @@
       </c>
       <c r="B1212" s="66"/>
       <c r="C1212" s="67" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="D1212" s="44">
         <f t="shared" si="66"/>
@@ -53255,7 +53250,7 @@
       </c>
       <c r="B1213" s="66"/>
       <c r="C1213" s="67" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="D1213" s="44">
         <f t="shared" si="66"/>
@@ -53291,7 +53286,7 @@
       </c>
       <c r="B1214" s="66"/>
       <c r="C1214" s="67" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="D1214" s="44">
         <f t="shared" si="66"/>
@@ -53327,7 +53322,7 @@
       </c>
       <c r="B1215" s="66"/>
       <c r="C1215" s="67" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="D1215" s="44">
         <f t="shared" si="66"/>
@@ -53363,7 +53358,7 @@
       </c>
       <c r="B1216" s="66"/>
       <c r="C1216" s="67" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="D1216" s="44">
         <f t="shared" si="66"/>
@@ -53401,7 +53396,7 @@
       </c>
       <c r="B1217" s="66"/>
       <c r="C1217" s="67" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="D1217" s="44">
         <f t="shared" si="66"/>
@@ -53439,7 +53434,7 @@
       </c>
       <c r="B1218" s="66"/>
       <c r="C1218" s="67" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="D1218" s="44">
         <f t="shared" si="66"/>
@@ -53475,7 +53470,7 @@
       </c>
       <c r="B1219" s="66"/>
       <c r="C1219" s="67" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="D1219" s="44">
         <f t="shared" si="66"/>
@@ -53511,7 +53506,7 @@
       </c>
       <c r="B1220" s="66"/>
       <c r="C1220" s="67" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="D1220" s="44">
         <f t="shared" si="66"/>
@@ -53547,7 +53542,7 @@
       </c>
       <c r="B1221" s="66"/>
       <c r="C1221" s="67" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="D1221" s="44">
         <f t="shared" si="66"/>
@@ -53583,7 +53578,7 @@
       </c>
       <c r="B1222" s="66"/>
       <c r="C1222" s="67" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="D1222" s="44">
         <f t="shared" ref="D1222:D1229" si="68">Q1222+O1222+M1222+K1222+I1222</f>
@@ -53621,7 +53616,7 @@
       </c>
       <c r="B1223" s="66"/>
       <c r="C1223" s="67" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="D1223" s="44">
         <f t="shared" si="68"/>
@@ -53659,7 +53654,7 @@
       </c>
       <c r="B1224" s="66"/>
       <c r="C1224" s="67" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="D1224" s="44">
         <f t="shared" si="68"/>
@@ -53695,7 +53690,7 @@
       </c>
       <c r="B1225" s="66"/>
       <c r="C1225" s="67" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="D1225" s="44">
         <f t="shared" si="68"/>
@@ -53731,7 +53726,7 @@
       </c>
       <c r="B1226" s="66"/>
       <c r="C1226" s="67" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="D1226" s="44">
         <f t="shared" si="68"/>
@@ -53767,7 +53762,7 @@
       </c>
       <c r="B1227" s="66"/>
       <c r="C1227" s="67" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="D1227" s="44">
         <f t="shared" si="68"/>
@@ -53805,7 +53800,7 @@
       </c>
       <c r="B1228" s="66"/>
       <c r="C1228" s="67" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="D1228" s="44">
         <f t="shared" si="68"/>
@@ -53841,7 +53836,7 @@
       </c>
       <c r="B1229" s="66"/>
       <c r="C1229" s="67" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="D1229" s="44">
         <f t="shared" si="68"/>
@@ -53877,7 +53872,7 @@
       </c>
       <c r="B1230" s="66"/>
       <c r="C1230" s="67" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="D1230" s="44">
         <f t="shared" ref="D1230:D1237" si="70">Q1230+O1230+M1230+K1230+I1230</f>
@@ -53915,7 +53910,7 @@
       </c>
       <c r="B1231" s="66"/>
       <c r="C1231" s="67" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="D1231" s="44">
         <f t="shared" si="70"/>
@@ -53951,7 +53946,7 @@
       </c>
       <c r="B1232" s="66"/>
       <c r="C1232" s="67" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="D1232" s="44">
         <f t="shared" si="70"/>
@@ -53987,7 +53982,7 @@
       </c>
       <c r="B1233" s="66"/>
       <c r="C1233" s="67" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="D1233" s="44">
         <f t="shared" si="70"/>
@@ -54023,7 +54018,7 @@
       </c>
       <c r="B1234" s="66"/>
       <c r="C1234" s="67" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="D1234" s="44">
         <f t="shared" si="70"/>
@@ -54059,7 +54054,7 @@
       </c>
       <c r="B1235" s="66"/>
       <c r="C1235" s="67" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="D1235" s="44">
         <f t="shared" si="70"/>
@@ -54095,7 +54090,7 @@
       </c>
       <c r="B1236" s="66"/>
       <c r="C1236" s="67" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="D1236" s="44">
         <f t="shared" si="70"/>
@@ -54131,7 +54126,7 @@
       </c>
       <c r="B1237" s="66"/>
       <c r="C1237" s="67" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="D1237" s="44">
         <f t="shared" si="70"/>
@@ -54208,7 +54203,7 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="D6:E743 D1208:E1221 D1222:E1229 D1230:E1230 D745:E1161 D1166:E1191 E1165 D1193:E1204 D1163:E1164 D1206:E1207" unlockedFormula="1"/>
+    <ignoredError sqref="D6:E743 D1208:E1221 D1222:E1229 D1230:E1230 D745:E860 D1166:E1191 E1165 D1193:E1204 D1163:E1164 D1206:E1207 D862:E1161" unlockedFormula="1"/>
     <ignoredError sqref="F6:F1208 F1210:F1229 F1231:F1304" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
@@ -54325,10 +54320,10 @@
         <v>6</v>
       </c>
       <c r="G4" s="73" t="s">
+        <v>1828</v>
+      </c>
+      <c r="H4" s="127" t="s">
         <v>1829</v>
-      </c>
-      <c r="H4" s="127" t="s">
-        <v>1830</v>
       </c>
       <c r="I4" s="74"/>
       <c r="J4" s="11" t="s">
@@ -59458,7 +59453,7 @@
       </c>
       <c r="B139" s="47"/>
       <c r="C139" s="82" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="D139" s="84">
         <f t="shared" si="8"/>
@@ -59497,7 +59492,7 @@
         <v>135</v>
       </c>
       <c r="C140" s="82" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="D140" s="84">
         <f t="shared" si="8"/>
@@ -59536,7 +59531,7 @@
         <v>136</v>
       </c>
       <c r="C141" s="82" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="D141" s="84">
         <f t="shared" si="8"/>
@@ -59573,7 +59568,7 @@
       </c>
       <c r="B142" s="47"/>
       <c r="C142" s="82" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="D142" s="84">
         <f t="shared" si="8"/>
@@ -59610,7 +59605,7 @@
       </c>
       <c r="B143" s="47"/>
       <c r="C143" s="82" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="D143" s="84">
         <f t="shared" si="8"/>
@@ -59647,7 +59642,7 @@
       </c>
       <c r="B144" s="47"/>
       <c r="C144" s="82" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="D144" s="84">
         <f t="shared" si="8"/>
@@ -59684,7 +59679,7 @@
       </c>
       <c r="B145" s="47"/>
       <c r="C145" s="82" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="D145" s="84">
         <f t="shared" si="8"/>
@@ -59723,7 +59718,7 @@
       </c>
       <c r="B146" s="47"/>
       <c r="C146" s="82" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="D146" s="84">
         <f t="shared" si="8"/>
@@ -59760,7 +59755,7 @@
       </c>
       <c r="B147" s="47"/>
       <c r="C147" s="82" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="D147" s="84">
         <f t="shared" si="8"/>
@@ -59797,7 +59792,7 @@
       </c>
       <c r="B148" s="47"/>
       <c r="C148" s="82" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="D148" s="84">
         <f t="shared" si="8"/>
@@ -59836,7 +59831,7 @@
       </c>
       <c r="B149" s="47"/>
       <c r="C149" s="82" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="D149" s="84">
         <f t="shared" si="8"/>
@@ -59873,7 +59868,7 @@
       </c>
       <c r="B150" s="47"/>
       <c r="C150" s="82" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="D150" s="84">
         <f t="shared" si="8"/>
@@ -59910,7 +59905,7 @@
       </c>
       <c r="B151" s="47"/>
       <c r="C151" s="82" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="D151" s="84">
         <f t="shared" si="8"/>
@@ -59951,7 +59946,7 @@
       </c>
       <c r="B152" s="47"/>
       <c r="C152" s="82" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="D152" s="84">
         <f t="shared" si="8"/>
@@ -59988,7 +59983,7 @@
       </c>
       <c r="B153" s="47"/>
       <c r="C153" s="82" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="D153" s="84">
         <f t="shared" si="8"/>
@@ -60025,7 +60020,7 @@
       </c>
       <c r="B154" s="47"/>
       <c r="C154" s="82" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="D154" s="84">
         <f t="shared" si="8"/>
@@ -60062,7 +60057,7 @@
       </c>
       <c r="B155" s="47"/>
       <c r="C155" s="82" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="D155" s="84">
         <f t="shared" si="8"/>
@@ -60099,7 +60094,7 @@
       </c>
       <c r="B156" s="47"/>
       <c r="C156" s="82" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="D156" s="84">
         <f t="shared" si="8"/>
@@ -60136,7 +60131,7 @@
       </c>
       <c r="B157" s="47"/>
       <c r="C157" s="82" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="D157" s="84">
         <f t="shared" si="8"/>
@@ -60173,7 +60168,7 @@
       </c>
       <c r="B158" s="47"/>
       <c r="C158" s="82" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="D158" s="84">
         <f t="shared" si="8"/>
@@ -60210,7 +60205,7 @@
       </c>
       <c r="B159" s="47"/>
       <c r="C159" s="82" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="D159" s="84">
         <f t="shared" si="8"/>
@@ -60249,7 +60244,7 @@
       </c>
       <c r="B160" s="47"/>
       <c r="C160" s="82" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="D160" s="84">
         <f t="shared" si="8"/>
@@ -60286,7 +60281,7 @@
       </c>
       <c r="B161" s="47"/>
       <c r="C161" s="82" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="D161" s="84">
         <f t="shared" si="8"/>
@@ -60323,7 +60318,7 @@
       </c>
       <c r="B162" s="2"/>
       <c r="C162" s="2" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="D162" s="84">
         <f t="shared" si="8"/>

</xml_diff>

<commit_message>
chore: update son sang oto
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E8AD74-6595-D746-AD16-3618406293BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A652F60E-8EDC-8843-AB33-B44F89C6B35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27700" yWindow="2660" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1971" uniqueCount="1896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="1916">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -5759,6 +5759,66 @@
   </si>
   <si>
     <t xml:space="preserve">Rin Hoàng Long </t>
+  </si>
+  <si>
+    <t>phú bánh mì</t>
+  </si>
+  <si>
+    <t>hào em</t>
+  </si>
+  <si>
+    <t>tony minh</t>
+  </si>
+  <si>
+    <t>tùng lương y</t>
+  </si>
+  <si>
+    <t>Long Tống</t>
+  </si>
+  <si>
+    <t>Khánh BK</t>
+  </si>
+  <si>
+    <t>Thành Thanh Đa</t>
+  </si>
+  <si>
+    <t>Tùng Sport</t>
+  </si>
+  <si>
+    <t>Cường Trà Vinh</t>
+  </si>
+  <si>
+    <t>Nu Trung Thiện</t>
+  </si>
+  <si>
+    <t>Hà Khanh BDS</t>
+  </si>
+  <si>
+    <t>Phước SPVB</t>
+  </si>
+  <si>
+    <t>Cường Riverside</t>
+  </si>
+  <si>
+    <t>Đông Nguyễn</t>
+  </si>
+  <si>
+    <t>Đình Điểm</t>
+  </si>
+  <si>
+    <t>Lâm Võ Sư</t>
+  </si>
+  <si>
+    <t>Hưng Cầu Dừa</t>
+  </si>
+  <si>
+    <t>Tùng Bình Dương</t>
+  </si>
+  <si>
+    <t>Xuân PVOIL</t>
+  </si>
+  <si>
+    <t>Khôi Q2</t>
   </si>
 </sst>
 </file>
@@ -7883,11 +7943,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R1237"/>
+  <dimension ref="A1:U1253"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A850" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I861" sqref="I861"/>
+      <pane ySplit="5" topLeftCell="A1229" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R1237" sqref="R1237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7910,7 +7970,7 @@
     <col min="19" max="16384" width="11.1640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="137" t="s">
         <v>0</v>
       </c>
@@ -7925,8 +7985,14 @@
       <c r="J1" s="29"/>
       <c r="K1" s="29"/>
       <c r="L1" s="29"/>
-    </row>
-    <row r="2" spans="1:18" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S1" s="32" t="s">
+        <v>1896</v>
+      </c>
+      <c r="U1" s="32" t="s">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="139" t="s">
         <v>1</v>
       </c>
@@ -7941,8 +8007,11 @@
       <c r="J2" s="29"/>
       <c r="K2" s="29"/>
       <c r="L2" s="29"/>
-    </row>
-    <row r="3" spans="1:18" s="109" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S2" s="33" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="109" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="107"/>
       <c r="B3" s="107"/>
       <c r="C3" s="107"/>
@@ -7957,8 +8026,11 @@
       <c r="L3" s="107"/>
       <c r="Q3" s="108"/>
       <c r="R3" s="108"/>
-    </row>
-    <row r="4" spans="1:18" s="110" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S3" s="109" t="s">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="110" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="105" t="s">
         <v>2</v>
       </c>
@@ -8000,7 +8072,7 @@
       </c>
       <c r="R4" s="142"/>
     </row>
-    <row r="5" spans="1:18" s="104" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" s="104" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="98"/>
       <c r="B5" s="98"/>
       <c r="C5" s="98"/>
@@ -8044,7 +8116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="26">
         <v>1</v>
       </c>
@@ -8056,7 +8128,7 @@
       </c>
       <c r="D6" s="44">
         <f>Q6+O6+M6+K6+I6</f>
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="E6" s="44">
         <f>P6+R6+N6+L6+J6</f>
@@ -8070,7 +8142,7 @@
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="112">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="J6" s="112"/>
       <c r="K6" s="96">
@@ -8092,7 +8164,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="26">
         <v>2</v>
       </c>
@@ -8132,7 +8204,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="26">
         <v>3</v>
       </c>
@@ -8182,7 +8254,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26">
         <v>4</v>
       </c>
@@ -8194,7 +8266,7 @@
       </c>
       <c r="D9" s="44">
         <f t="shared" si="0"/>
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="E9" s="44">
         <f t="shared" si="1"/>
@@ -8207,7 +8279,9 @@
         <v>1</v>
       </c>
       <c r="H9" s="14"/>
-      <c r="I9" s="112"/>
+      <c r="I9" s="112">
+        <v>-5</v>
+      </c>
       <c r="J9" s="112"/>
       <c r="K9" s="96"/>
       <c r="L9" s="96"/>
@@ -8224,7 +8298,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="26">
         <v>5</v>
       </c>
@@ -8264,7 +8338,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="26">
         <v>6</v>
       </c>
@@ -8300,7 +8374,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="26">
         <v>7</v>
       </c>
@@ -8336,7 +8410,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="26">
         <v>8</v>
       </c>
@@ -8374,7 +8448,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="26">
         <v>9</v>
       </c>
@@ -8412,7 +8486,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="26">
         <v>10</v>
       </c>
@@ -8456,7 +8530,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="26">
         <v>11</v>
       </c>
@@ -8732,7 +8806,7 @@
       </c>
       <c r="D23" s="44">
         <f t="shared" si="0"/>
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="E23" s="44">
         <f t="shared" si="1"/>
@@ -8745,7 +8819,9 @@
         <v>1</v>
       </c>
       <c r="H23" s="14"/>
-      <c r="I23" s="112"/>
+      <c r="I23" s="112">
+        <v>-5</v>
+      </c>
       <c r="J23" s="112"/>
       <c r="K23" s="96"/>
       <c r="L23" s="96"/>
@@ -8856,7 +8932,7 @@
       </c>
       <c r="D26" s="44">
         <f t="shared" si="0"/>
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="E26" s="44">
         <f t="shared" si="1"/>
@@ -8867,7 +8943,9 @@
         <v>1</v>
       </c>
       <c r="H26" s="14"/>
-      <c r="I26" s="112"/>
+      <c r="I26" s="112">
+        <v>-5</v>
+      </c>
       <c r="J26" s="112"/>
       <c r="K26" s="96"/>
       <c r="L26" s="96"/>
@@ -9046,7 +9124,7 @@
       </c>
       <c r="D31" s="44">
         <f t="shared" si="0"/>
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="E31" s="44">
         <f t="shared" si="1"/>
@@ -9059,7 +9137,9 @@
         <v>1</v>
       </c>
       <c r="H31" s="14"/>
-      <c r="I31" s="112"/>
+      <c r="I31" s="112">
+        <v>5</v>
+      </c>
       <c r="J31" s="112"/>
       <c r="K31" s="96"/>
       <c r="L31" s="96"/>
@@ -9708,7 +9788,7 @@
       </c>
       <c r="D48" s="44">
         <f t="shared" si="0"/>
-        <v>635</v>
+        <v>640</v>
       </c>
       <c r="E48" s="44">
         <f t="shared" si="1"/>
@@ -9722,7 +9802,7 @@
       </c>
       <c r="H48" s="14"/>
       <c r="I48" s="112">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J48" s="112"/>
       <c r="K48" s="96">
@@ -10010,7 +10090,7 @@
       </c>
       <c r="D56" s="44">
         <f t="shared" si="0"/>
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="E56" s="44">
         <f t="shared" si="1"/>
@@ -10022,7 +10102,7 @@
       </c>
       <c r="H56" s="24"/>
       <c r="I56" s="113">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="J56" s="113"/>
       <c r="K56" s="96"/>
@@ -10090,19 +10170,23 @@
       </c>
       <c r="D58" s="44">
         <f t="shared" si="0"/>
-        <v>680</v>
+        <v>695</v>
       </c>
       <c r="E58" s="44">
         <f t="shared" si="1"/>
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="F58" s="47"/>
       <c r="G58" s="47">
         <v>1</v>
       </c>
       <c r="H58" s="14"/>
-      <c r="I58" s="112"/>
-      <c r="J58" s="112"/>
+      <c r="I58" s="112">
+        <v>15</v>
+      </c>
+      <c r="J58" s="112">
+        <v>5</v>
+      </c>
       <c r="K58" s="96">
         <v>-5</v>
       </c>
@@ -10448,7 +10532,7 @@
       </c>
       <c r="D67" s="44">
         <f t="shared" si="0"/>
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="E67" s="44">
         <f t="shared" si="1"/>
@@ -10459,7 +10543,9 @@
         <v>1</v>
       </c>
       <c r="H67" s="14"/>
-      <c r="I67" s="112"/>
+      <c r="I67" s="112">
+        <v>-5</v>
+      </c>
       <c r="J67" s="112"/>
       <c r="K67" s="96"/>
       <c r="L67" s="96"/>
@@ -11436,7 +11522,7 @@
       </c>
       <c r="D93" s="44">
         <f t="shared" si="6"/>
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="E93" s="44">
         <f t="shared" si="7"/>
@@ -11449,7 +11535,9 @@
         <v>1</v>
       </c>
       <c r="H93" s="14"/>
-      <c r="I93" s="112"/>
+      <c r="I93" s="112">
+        <v>-5</v>
+      </c>
       <c r="J93" s="112"/>
       <c r="K93" s="96"/>
       <c r="L93" s="96"/>
@@ -12124,7 +12212,7 @@
       </c>
       <c r="D111" s="44">
         <f t="shared" si="8"/>
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E111" s="44">
         <f t="shared" si="9"/>
@@ -12135,7 +12223,9 @@
         <v>1</v>
       </c>
       <c r="H111" s="14"/>
-      <c r="I111" s="112"/>
+      <c r="I111" s="112">
+        <v>-5</v>
+      </c>
       <c r="J111" s="112">
         <v>-5</v>
       </c>
@@ -12166,7 +12256,7 @@
       </c>
       <c r="E112" s="44">
         <f t="shared" si="9"/>
-        <v>725</v>
+        <v>710</v>
       </c>
       <c r="F112" s="47"/>
       <c r="G112" s="47">
@@ -12174,7 +12264,9 @@
       </c>
       <c r="H112" s="14"/>
       <c r="I112" s="112"/>
-      <c r="J112" s="112"/>
+      <c r="J112" s="112">
+        <v>-15</v>
+      </c>
       <c r="K112" s="96"/>
       <c r="L112" s="96"/>
       <c r="M112" s="76"/>
@@ -12198,11 +12290,11 @@
       </c>
       <c r="D113" s="44">
         <f t="shared" si="8"/>
-        <v>595</v>
+        <v>610</v>
       </c>
       <c r="E113" s="44">
         <f t="shared" si="9"/>
-        <v>590</v>
+        <v>600</v>
       </c>
       <c r="F113" s="47"/>
       <c r="G113" s="47">
@@ -12210,10 +12302,10 @@
       </c>
       <c r="H113" s="14"/>
       <c r="I113" s="112">
-        <v>-5</v>
+        <v>10</v>
       </c>
       <c r="J113" s="112">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="K113" s="96"/>
       <c r="L113" s="96"/>
@@ -12274,7 +12366,7 @@
       </c>
       <c r="D115" s="44">
         <f t="shared" si="8"/>
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="E115" s="44">
         <f t="shared" si="9"/>
@@ -12285,7 +12377,9 @@
         <v>1</v>
       </c>
       <c r="H115" s="48"/>
-      <c r="I115" s="112"/>
+      <c r="I115" s="112">
+        <v>-5</v>
+      </c>
       <c r="J115" s="112"/>
       <c r="K115" s="96"/>
       <c r="L115" s="96"/>
@@ -12737,7 +12831,7 @@
       </c>
       <c r="D127" s="44">
         <f t="shared" si="8"/>
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="E127" s="44">
         <f t="shared" si="9"/>
@@ -12748,7 +12842,9 @@
         <v>1</v>
       </c>
       <c r="H127" s="24"/>
-      <c r="I127" s="113"/>
+      <c r="I127" s="113">
+        <v>-5</v>
+      </c>
       <c r="J127" s="113"/>
       <c r="K127" s="96">
         <v>-5</v>
@@ -12777,7 +12873,7 @@
       </c>
       <c r="D128" s="44">
         <f t="shared" si="8"/>
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="E128" s="44">
         <f t="shared" si="9"/>
@@ -12790,7 +12886,9 @@
         <v>1</v>
       </c>
       <c r="H128" s="14"/>
-      <c r="I128" s="112"/>
+      <c r="I128" s="112">
+        <v>-5</v>
+      </c>
       <c r="J128" s="112"/>
       <c r="K128" s="96">
         <v>15</v>
@@ -16321,11 +16419,11 @@
       </c>
       <c r="D222" s="44">
         <f t="shared" si="16"/>
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="E222" s="44">
         <f t="shared" si="17"/>
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="F222" s="50" t="s">
         <v>1552</v>
@@ -16334,8 +16432,12 @@
         <v>1</v>
       </c>
       <c r="H222" s="14"/>
-      <c r="I222" s="112"/>
-      <c r="J222" s="112"/>
+      <c r="I222" s="112">
+        <v>-5</v>
+      </c>
+      <c r="J222" s="112">
+        <v>-5</v>
+      </c>
       <c r="K222" s="96"/>
       <c r="L222" s="96"/>
       <c r="M222" s="76"/>
@@ -17607,7 +17709,7 @@
       </c>
       <c r="D256" s="44">
         <f t="shared" si="18"/>
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="E256" s="44">
         <f t="shared" si="19"/>
@@ -17620,7 +17722,9 @@
         <v>1</v>
       </c>
       <c r="H256" s="14"/>
-      <c r="I256" s="112"/>
+      <c r="I256" s="112">
+        <v>-5</v>
+      </c>
       <c r="J256" s="112"/>
       <c r="K256" s="96"/>
       <c r="L256" s="96"/>
@@ -18393,7 +18497,7 @@
       </c>
       <c r="D277" s="44">
         <f t="shared" si="18"/>
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="E277" s="44">
         <f t="shared" si="19"/>
@@ -18406,7 +18510,9 @@
         <v>1</v>
       </c>
       <c r="H277" s="14"/>
-      <c r="I277" s="112"/>
+      <c r="I277" s="112">
+        <v>-5</v>
+      </c>
       <c r="J277" s="112"/>
       <c r="K277" s="96"/>
       <c r="L277" s="96"/>
@@ -18431,7 +18537,7 @@
       </c>
       <c r="D278" s="44">
         <f t="shared" si="18"/>
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="E278" s="44">
         <f t="shared" si="19"/>
@@ -18444,7 +18550,9 @@
         <v>1</v>
       </c>
       <c r="H278" s="14"/>
-      <c r="I278" s="112"/>
+      <c r="I278" s="112">
+        <v>-5</v>
+      </c>
       <c r="J278" s="112"/>
       <c r="K278" s="96"/>
       <c r="L278" s="96"/>
@@ -22467,7 +22575,7 @@
       </c>
       <c r="D385" s="44">
         <f t="shared" si="24"/>
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="E385" s="44">
         <f t="shared" si="25"/>
@@ -22478,7 +22586,9 @@
         <v>1</v>
       </c>
       <c r="H385" s="48"/>
-      <c r="I385" s="115"/>
+      <c r="I385" s="115">
+        <v>-5</v>
+      </c>
       <c r="J385" s="115"/>
       <c r="K385" s="96"/>
       <c r="L385" s="96"/>
@@ -24255,19 +24365,23 @@
       </c>
       <c r="D433" s="44">
         <f t="shared" si="28"/>
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="E433" s="44">
         <f t="shared" si="29"/>
-        <v>660</v>
+        <v>640</v>
       </c>
       <c r="F433" s="47"/>
       <c r="G433" s="47">
         <v>1</v>
       </c>
       <c r="H433" s="14"/>
-      <c r="I433" s="112"/>
-      <c r="J433" s="112"/>
+      <c r="I433" s="112">
+        <v>-5</v>
+      </c>
+      <c r="J433" s="112">
+        <v>-20</v>
+      </c>
       <c r="K433" s="96"/>
       <c r="L433" s="96"/>
       <c r="M433" s="76">
@@ -24333,7 +24447,7 @@
       </c>
       <c r="E435" s="44">
         <f t="shared" si="29"/>
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="F435" s="45" t="s">
         <v>552</v>
@@ -24343,7 +24457,9 @@
       </c>
       <c r="H435" s="14"/>
       <c r="I435" s="112"/>
-      <c r="J435" s="112"/>
+      <c r="J435" s="112">
+        <v>-5</v>
+      </c>
       <c r="K435" s="96"/>
       <c r="L435" s="96"/>
       <c r="M435" s="76"/>
@@ -25921,7 +26037,7 @@
       </c>
       <c r="D478" s="44">
         <f t="shared" si="30"/>
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="E478" s="44">
         <f t="shared" si="31"/>
@@ -25934,7 +26050,9 @@
         <v>1</v>
       </c>
       <c r="H478" s="52"/>
-      <c r="I478" s="116"/>
+      <c r="I478" s="116">
+        <v>-5</v>
+      </c>
       <c r="J478" s="116"/>
       <c r="K478" s="96">
         <v>-5</v>
@@ -26387,11 +26505,11 @@
       </c>
       <c r="D490" s="44">
         <f t="shared" si="30"/>
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E490" s="44">
         <f t="shared" si="31"/>
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="F490" s="47"/>
       <c r="G490" s="47">
@@ -26399,10 +26517,10 @@
       </c>
       <c r="H490" s="14"/>
       <c r="I490" s="129">
-        <v>-10</v>
+        <v>-15</v>
       </c>
       <c r="J490" s="129">
-        <v>-10</v>
+        <v>-15</v>
       </c>
       <c r="K490" s="96"/>
       <c r="L490" s="96"/>
@@ -27847,7 +27965,7 @@
       </c>
       <c r="D529" s="44">
         <f t="shared" si="36"/>
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="E529" s="44">
         <f t="shared" si="37"/>
@@ -27861,7 +27979,7 @@
       </c>
       <c r="H529" s="14"/>
       <c r="I529" s="112">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J529" s="112"/>
       <c r="K529" s="96"/>
@@ -28105,19 +28223,23 @@
       </c>
       <c r="D536" s="44">
         <f t="shared" si="36"/>
-        <v>680</v>
+        <v>670</v>
       </c>
       <c r="E536" s="44">
         <f t="shared" si="37"/>
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="F536" s="47"/>
       <c r="G536" s="47">
         <v>1</v>
       </c>
       <c r="H536" s="14"/>
-      <c r="I536" s="112"/>
-      <c r="J536" s="112"/>
+      <c r="I536" s="112">
+        <v>-10</v>
+      </c>
+      <c r="J536" s="112">
+        <v>-10</v>
+      </c>
       <c r="K536" s="96">
         <v>-5</v>
       </c>
@@ -30919,11 +31041,11 @@
       </c>
       <c r="D611" s="44">
         <f t="shared" si="38"/>
-        <v>620</v>
+        <v>630</v>
       </c>
       <c r="E611" s="44">
         <f t="shared" si="39"/>
-        <v>615</v>
+        <v>620</v>
       </c>
       <c r="F611" s="45" t="s">
         <v>803</v>
@@ -30932,8 +31054,12 @@
         <v>1</v>
       </c>
       <c r="H611" s="48"/>
-      <c r="I611" s="115"/>
-      <c r="J611" s="115"/>
+      <c r="I611" s="115">
+        <v>10</v>
+      </c>
+      <c r="J611" s="115">
+        <v>5</v>
+      </c>
       <c r="K611" s="96"/>
       <c r="L611" s="96"/>
       <c r="M611" s="77"/>
@@ -34315,11 +34441,11 @@
       </c>
       <c r="D702" s="44">
         <f t="shared" ref="D702:D743" si="42">Q702+O702+M702+K702+I702</f>
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="E702" s="44">
         <f t="shared" ref="E702:E743" si="43">P702+R702+N702+L702+J702</f>
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="F702" s="47"/>
       <c r="G702" s="47">
@@ -34327,9 +34453,11 @@
       </c>
       <c r="H702" s="14"/>
       <c r="I702" s="129">
+        <v>-10</v>
+      </c>
+      <c r="J702" s="112">
         <v>-5</v>
       </c>
-      <c r="J702" s="112"/>
       <c r="K702" s="96"/>
       <c r="L702" s="96"/>
       <c r="M702" s="76"/>
@@ -35119,20 +35247,22 @@
       </c>
       <c r="D724" s="44">
         <f t="shared" si="42"/>
-        <v>605</v>
+        <v>620</v>
       </c>
       <c r="E724" s="44">
         <f t="shared" si="43"/>
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="F724" s="47"/>
       <c r="G724" s="47">
         <v>1</v>
       </c>
       <c r="H724" s="14"/>
-      <c r="I724" s="112"/>
+      <c r="I724" s="112">
+        <v>15</v>
+      </c>
       <c r="J724" s="112">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K724" s="96">
         <v>-5</v>
@@ -35813,19 +35943,23 @@
       </c>
       <c r="D743" s="44">
         <f t="shared" si="42"/>
-        <v>620</v>
+        <v>635</v>
       </c>
       <c r="E743" s="44">
         <f t="shared" si="43"/>
-        <v>620</v>
+        <v>625</v>
       </c>
       <c r="F743" s="47"/>
       <c r="G743" s="47">
         <v>1</v>
       </c>
       <c r="H743" s="14"/>
-      <c r="I743" s="112"/>
-      <c r="J743" s="112"/>
+      <c r="I743" s="112">
+        <v>15</v>
+      </c>
+      <c r="J743" s="112">
+        <v>5</v>
+      </c>
       <c r="K743" s="96"/>
       <c r="L743" s="96"/>
       <c r="M743" s="76"/>
@@ -36241,7 +36375,7 @@
       </c>
       <c r="D755" s="44">
         <f t="shared" si="44"/>
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="E755" s="44">
         <f t="shared" si="45"/>
@@ -36252,7 +36386,9 @@
         <v>1</v>
       </c>
       <c r="H755" s="14"/>
-      <c r="I755" s="112"/>
+      <c r="I755" s="112">
+        <v>-5</v>
+      </c>
       <c r="J755" s="112"/>
       <c r="K755" s="96"/>
       <c r="L755" s="96"/>
@@ -36423,19 +36559,23 @@
       </c>
       <c r="D760" s="44">
         <f t="shared" si="44"/>
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="E760" s="44">
         <f t="shared" si="45"/>
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="F760" s="47"/>
       <c r="G760" s="47">
         <v>1</v>
       </c>
       <c r="H760" s="14"/>
-      <c r="I760" s="112"/>
-      <c r="J760" s="112"/>
+      <c r="I760" s="112">
+        <v>-5</v>
+      </c>
+      <c r="J760" s="112">
+        <v>-5</v>
+      </c>
       <c r="K760" s="96"/>
       <c r="L760" s="96"/>
       <c r="M760" s="76">
@@ -37067,11 +37207,11 @@
       </c>
       <c r="D777" s="44">
         <f t="shared" si="44"/>
-        <v>670</v>
+        <v>675</v>
       </c>
       <c r="E777" s="44">
         <f t="shared" si="45"/>
-        <v>650</v>
+        <v>660</v>
       </c>
       <c r="F777" s="47" t="s">
         <v>1260</v>
@@ -37080,8 +37220,12 @@
         <v>1</v>
       </c>
       <c r="H777" s="14"/>
-      <c r="I777" s="112"/>
-      <c r="J777" s="112"/>
+      <c r="I777" s="112">
+        <v>5</v>
+      </c>
+      <c r="J777" s="112">
+        <v>10</v>
+      </c>
       <c r="K777" s="96"/>
       <c r="L777" s="96"/>
       <c r="M777" s="76"/>
@@ -37861,7 +38005,7 @@
       </c>
       <c r="E798" s="44">
         <f t="shared" si="45"/>
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="F798" s="47"/>
       <c r="G798" s="47">
@@ -37869,7 +38013,9 @@
       </c>
       <c r="H798" s="14"/>
       <c r="I798" s="112"/>
-      <c r="J798" s="112"/>
+      <c r="J798" s="112">
+        <v>-10</v>
+      </c>
       <c r="K798" s="96"/>
       <c r="L798" s="96"/>
       <c r="M798" s="76"/>
@@ -38079,7 +38225,7 @@
       </c>
       <c r="D804" s="44">
         <f t="shared" si="44"/>
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="E804" s="44">
         <f t="shared" si="45"/>
@@ -38090,7 +38236,9 @@
         <v>1</v>
       </c>
       <c r="H804" s="14"/>
-      <c r="I804" s="112"/>
+      <c r="I804" s="112">
+        <v>-5</v>
+      </c>
       <c r="J804" s="112"/>
       <c r="K804" s="96"/>
       <c r="L804" s="96"/>
@@ -38489,7 +38637,7 @@
       </c>
       <c r="D815" s="44">
         <f t="shared" si="46"/>
-        <v>590</v>
+        <v>600</v>
       </c>
       <c r="E815" s="44">
         <f t="shared" si="47"/>
@@ -38500,7 +38648,9 @@
         <v>1</v>
       </c>
       <c r="H815" s="14"/>
-      <c r="I815" s="112"/>
+      <c r="I815" s="112">
+        <v>10</v>
+      </c>
       <c r="J815" s="112"/>
       <c r="K815" s="96"/>
       <c r="L815" s="96"/>
@@ -39051,7 +39201,7 @@
       </c>
       <c r="D830" s="44">
         <f t="shared" si="46"/>
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="E830" s="44">
         <f t="shared" si="47"/>
@@ -39062,7 +39212,9 @@
         <v>1</v>
       </c>
       <c r="H830" s="14"/>
-      <c r="I830" s="112"/>
+      <c r="I830" s="112">
+        <v>-5</v>
+      </c>
       <c r="J830" s="112"/>
       <c r="K830" s="96"/>
       <c r="L830" s="96"/>
@@ -39987,7 +40139,7 @@
       </c>
       <c r="D855" s="44">
         <f t="shared" si="46"/>
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="E855" s="44">
         <f t="shared" si="47"/>
@@ -40000,7 +40152,9 @@
         <v>1</v>
       </c>
       <c r="H855" s="14"/>
-      <c r="I855" s="112"/>
+      <c r="I855" s="112">
+        <v>-5</v>
+      </c>
       <c r="J855" s="112">
         <v>-10</v>
       </c>
@@ -41829,7 +41983,7 @@
       </c>
       <c r="D905" s="44">
         <f t="shared" si="48"/>
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="E905" s="44">
         <f t="shared" si="49"/>
@@ -41841,7 +41995,7 @@
       </c>
       <c r="H905" s="13"/>
       <c r="I905" s="117">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J905" s="117"/>
       <c r="K905" s="96"/>
@@ -41871,7 +42025,7 @@
       </c>
       <c r="D906" s="44">
         <f t="shared" si="48"/>
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="E906" s="44">
         <f t="shared" si="49"/>
@@ -41882,7 +42036,9 @@
         <v>1</v>
       </c>
       <c r="H906" s="13"/>
-      <c r="I906" s="117"/>
+      <c r="I906" s="117">
+        <v>-5</v>
+      </c>
       <c r="J906" s="117"/>
       <c r="K906" s="96"/>
       <c r="L906" s="96"/>
@@ -41907,7 +42063,7 @@
       </c>
       <c r="D907" s="44">
         <f t="shared" si="48"/>
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="E907" s="44">
         <f t="shared" si="49"/>
@@ -41919,7 +42075,7 @@
       </c>
       <c r="H907" s="13"/>
       <c r="I907" s="117">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J907" s="117"/>
       <c r="K907" s="96">
@@ -41987,19 +42143,23 @@
       </c>
       <c r="D909" s="44">
         <f t="shared" si="48"/>
-        <v>695</v>
+        <v>705</v>
       </c>
       <c r="E909" s="44">
         <f t="shared" si="49"/>
-        <v>680</v>
+        <v>700</v>
       </c>
       <c r="F909" s="47"/>
       <c r="G909" s="47">
         <v>1</v>
       </c>
       <c r="H909" s="13"/>
-      <c r="I909" s="117"/>
-      <c r="J909" s="117"/>
+      <c r="I909" s="117">
+        <v>10</v>
+      </c>
+      <c r="J909" s="117">
+        <v>20</v>
+      </c>
       <c r="K909" s="96"/>
       <c r="L909" s="96"/>
       <c r="M909" s="76">
@@ -42025,7 +42185,7 @@
       </c>
       <c r="D910" s="44">
         <f t="shared" si="48"/>
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="E910" s="44">
         <f t="shared" si="49"/>
@@ -42036,7 +42196,9 @@
         <v>1</v>
       </c>
       <c r="H910" s="13"/>
-      <c r="I910" s="117"/>
+      <c r="I910" s="117">
+        <v>-5</v>
+      </c>
       <c r="J910" s="117"/>
       <c r="K910" s="96"/>
       <c r="L910" s="96"/>
@@ -42133,19 +42295,23 @@
       </c>
       <c r="D913" s="44">
         <f t="shared" si="48"/>
-        <v>615</v>
+        <v>630</v>
       </c>
       <c r="E913" s="44">
         <f t="shared" si="49"/>
-        <v>610</v>
+        <v>620</v>
       </c>
       <c r="F913" s="47"/>
       <c r="G913" s="47">
         <v>1</v>
       </c>
       <c r="H913" s="13"/>
-      <c r="I913" s="117"/>
-      <c r="J913" s="117"/>
+      <c r="I913" s="117">
+        <v>15</v>
+      </c>
+      <c r="J913" s="117">
+        <v>10</v>
+      </c>
       <c r="K913" s="96"/>
       <c r="L913" s="96"/>
       <c r="M913" s="76"/>
@@ -42595,7 +42761,7 @@
       </c>
       <c r="E925" s="44">
         <f t="shared" si="49"/>
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="F925" s="54" t="s">
         <v>1477</v>
@@ -42605,7 +42771,9 @@
       </c>
       <c r="H925" s="55"/>
       <c r="I925" s="118"/>
-      <c r="J925" s="118"/>
+      <c r="J925" s="118">
+        <v>-5</v>
+      </c>
       <c r="K925" s="96"/>
       <c r="L925" s="96"/>
       <c r="M925" s="79">
@@ -43053,7 +43221,7 @@
       </c>
       <c r="D937" s="44">
         <f t="shared" ref="D937:D1000" si="50">Q937+O937+M937+K937+I937</f>
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="E937" s="44">
         <f t="shared" ref="E937:E1000" si="51">P937+R937+N937+L937+J937</f>
@@ -43064,7 +43232,9 @@
         <v>1</v>
       </c>
       <c r="H937" s="13"/>
-      <c r="I937" s="117"/>
+      <c r="I937" s="117">
+        <v>5</v>
+      </c>
       <c r="J937" s="117"/>
       <c r="K937" s="96"/>
       <c r="L937" s="96"/>
@@ -43461,7 +43631,7 @@
       </c>
       <c r="E947" s="44">
         <f t="shared" si="51"/>
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="F947" s="47"/>
       <c r="G947" s="47">
@@ -43469,7 +43639,9 @@
       </c>
       <c r="H947" s="13"/>
       <c r="I947" s="117"/>
-      <c r="J947" s="117"/>
+      <c r="J947" s="117">
+        <v>-5</v>
+      </c>
       <c r="K947" s="96"/>
       <c r="L947" s="96"/>
       <c r="M947" s="76"/>
@@ -44189,7 +44361,7 @@
       </c>
       <c r="D967" s="44">
         <f t="shared" si="50"/>
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="E967" s="44">
         <f t="shared" si="51"/>
@@ -44200,7 +44372,9 @@
         <v>1</v>
       </c>
       <c r="H967" s="13"/>
-      <c r="I967" s="117"/>
+      <c r="I967" s="117">
+        <v>-5</v>
+      </c>
       <c r="J967" s="117"/>
       <c r="K967" s="96"/>
       <c r="L967" s="96"/>
@@ -45153,19 +45327,23 @@
       </c>
       <c r="D993" s="44">
         <f t="shared" si="50"/>
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="E993" s="44">
         <f t="shared" si="51"/>
-        <v>590</v>
+        <v>600</v>
       </c>
       <c r="F993" s="47"/>
       <c r="G993" s="47">
         <v>1</v>
       </c>
       <c r="H993" s="13"/>
-      <c r="I993" s="117"/>
-      <c r="J993" s="117"/>
+      <c r="I993" s="117">
+        <v>5</v>
+      </c>
+      <c r="J993" s="117">
+        <v>10</v>
+      </c>
       <c r="K993" s="96"/>
       <c r="L993" s="96"/>
       <c r="M993" s="76"/>
@@ -45189,7 +45367,7 @@
       </c>
       <c r="D994" s="44">
         <f t="shared" si="50"/>
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="E994" s="44">
         <f t="shared" si="51"/>
@@ -45201,7 +45379,7 @@
       </c>
       <c r="H994" s="13"/>
       <c r="I994" s="117">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J994" s="117">
         <v>10</v>
@@ -46145,11 +46323,11 @@
       </c>
       <c r="D1020" s="44">
         <f t="shared" si="52"/>
-        <v>625</v>
+        <v>630</v>
       </c>
       <c r="E1020" s="44">
         <f t="shared" si="53"/>
-        <v>615</v>
+        <v>620</v>
       </c>
       <c r="F1020" s="47"/>
       <c r="G1020" s="47">
@@ -46157,9 +46335,11 @@
       </c>
       <c r="H1020" s="24"/>
       <c r="I1020" s="113">
+        <v>10</v>
+      </c>
+      <c r="J1020" s="113">
         <v>5</v>
       </c>
-      <c r="J1020" s="113"/>
       <c r="K1020" s="96">
         <v>10</v>
       </c>
@@ -48343,19 +48523,23 @@
       </c>
       <c r="D1080" s="44">
         <f t="shared" si="54"/>
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="E1080" s="44">
         <f t="shared" si="55"/>
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="F1080" s="34"/>
       <c r="G1080" s="47">
         <v>1</v>
       </c>
       <c r="H1080" s="17"/>
-      <c r="I1080" s="119"/>
-      <c r="J1080" s="119"/>
+      <c r="I1080" s="119">
+        <v>-5</v>
+      </c>
+      <c r="J1080" s="119">
+        <v>-5</v>
+      </c>
       <c r="K1080" s="96">
         <v>-5</v>
       </c>
@@ -50379,7 +50563,7 @@
       </c>
       <c r="D1135" s="44">
         <f t="shared" si="56"/>
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="E1135" s="44">
         <f t="shared" si="57"/>
@@ -50390,7 +50574,9 @@
         <v>1</v>
       </c>
       <c r="H1135" s="68"/>
-      <c r="I1135" s="119"/>
+      <c r="I1135" s="119">
+        <v>-5</v>
+      </c>
       <c r="J1135" s="119"/>
       <c r="K1135" s="96">
         <v>-5</v>
@@ -50688,19 +50874,23 @@
       </c>
       <c r="D1143" s="44">
         <f t="shared" si="56"/>
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="E1143" s="44">
         <f t="shared" si="57"/>
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="F1143" s="66"/>
       <c r="G1143" s="47">
         <v>1</v>
       </c>
       <c r="H1143" s="68"/>
-      <c r="I1143" s="119"/>
-      <c r="J1143" s="119"/>
+      <c r="I1143" s="119">
+        <v>-5</v>
+      </c>
+      <c r="J1143" s="119">
+        <v>-10</v>
+      </c>
       <c r="K1143" s="96"/>
       <c r="L1143" s="96"/>
       <c r="M1143" s="80"/>
@@ -51742,19 +51932,23 @@
       </c>
       <c r="D1172" s="44">
         <f t="shared" si="62"/>
-        <v>620</v>
+        <v>635</v>
       </c>
       <c r="E1172" s="44">
         <f t="shared" si="63"/>
-        <v>610</v>
+        <v>620</v>
       </c>
       <c r="F1172" s="66"/>
       <c r="G1172" s="47">
         <v>1</v>
       </c>
       <c r="H1172" s="68"/>
-      <c r="I1172" s="119"/>
-      <c r="J1172" s="119"/>
+      <c r="I1172" s="119">
+        <v>15</v>
+      </c>
+      <c r="J1172" s="119">
+        <v>10</v>
+      </c>
       <c r="K1172" s="96"/>
       <c r="L1172" s="96"/>
       <c r="M1172" s="80"/>
@@ -51922,11 +52116,11 @@
       </c>
       <c r="D1177" s="44">
         <f t="shared" si="62"/>
-        <v>610</v>
+        <v>625</v>
       </c>
       <c r="E1177" s="44">
         <f t="shared" si="63"/>
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="F1177" s="66"/>
       <c r="G1177" s="47">
@@ -51934,9 +52128,11 @@
       </c>
       <c r="H1177" s="68"/>
       <c r="I1177" s="119">
-        <v>-5</v>
-      </c>
-      <c r="J1177" s="119"/>
+        <v>10</v>
+      </c>
+      <c r="J1177" s="119">
+        <v>5</v>
+      </c>
       <c r="K1177" s="96"/>
       <c r="L1177" s="96"/>
       <c r="M1177" s="80"/>
@@ -53879,7 +54075,7 @@
         <v>615</v>
       </c>
       <c r="E1230" s="44">
-        <f t="shared" ref="E1230:E1237" si="71">P1230+R1230+N1230+L1230+J1230</f>
+        <f t="shared" ref="E1230:E1251" si="71">P1230+R1230+N1230+L1230+J1230</f>
         <v>610</v>
       </c>
       <c r="F1230" s="66"/>
@@ -54130,7 +54326,7 @@
       </c>
       <c r="D1237" s="44">
         <f t="shared" si="70"/>
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="E1237" s="44">
         <f t="shared" si="71"/>
@@ -54141,7 +54337,9 @@
         <v>1</v>
       </c>
       <c r="H1237" s="68"/>
-      <c r="I1237" s="119"/>
+      <c r="I1237" s="119">
+        <v>-5</v>
+      </c>
       <c r="J1237" s="119"/>
       <c r="K1237" s="96"/>
       <c r="L1237" s="96"/>
@@ -54154,6 +54352,582 @@
       </c>
       <c r="R1237" s="70">
         <v>700</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1238" s="1">
+        <v>1233</v>
+      </c>
+      <c r="B1238" s="66"/>
+      <c r="C1238" s="67" t="s">
+        <v>1900</v>
+      </c>
+      <c r="D1238" s="44">
+        <f t="shared" ref="D1238:D1253" si="72">Q1238+O1238+M1238+K1238+I1238</f>
+        <v>650</v>
+      </c>
+      <c r="E1238" s="44">
+        <f t="shared" ref="E1238:E1253" si="73">P1238+R1238+N1238+L1238+J1238</f>
+        <v>640</v>
+      </c>
+      <c r="F1238" s="66"/>
+      <c r="G1238" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1238" s="68"/>
+      <c r="I1238" s="119"/>
+      <c r="J1238" s="119"/>
+      <c r="K1238" s="96"/>
+      <c r="L1238" s="96"/>
+      <c r="M1238" s="80"/>
+      <c r="N1238" s="80"/>
+      <c r="O1238" s="69"/>
+      <c r="P1238" s="69"/>
+      <c r="Q1238" s="70">
+        <v>650</v>
+      </c>
+      <c r="R1238" s="70">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1239" s="1">
+        <v>1234</v>
+      </c>
+      <c r="B1239" s="66"/>
+      <c r="C1239" s="67" t="s">
+        <v>1901</v>
+      </c>
+      <c r="D1239" s="44">
+        <f t="shared" si="72"/>
+        <v>590</v>
+      </c>
+      <c r="E1239" s="44">
+        <f t="shared" si="73"/>
+        <v>585</v>
+      </c>
+      <c r="F1239" s="66"/>
+      <c r="G1239" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1239" s="68"/>
+      <c r="I1239" s="119"/>
+      <c r="J1239" s="119"/>
+      <c r="K1239" s="96"/>
+      <c r="L1239" s="96"/>
+      <c r="M1239" s="80"/>
+      <c r="N1239" s="80"/>
+      <c r="O1239" s="69"/>
+      <c r="P1239" s="69"/>
+      <c r="Q1239" s="70">
+        <v>590</v>
+      </c>
+      <c r="R1239" s="70">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1240" s="1">
+        <v>1235</v>
+      </c>
+      <c r="B1240" s="66"/>
+      <c r="C1240" s="67" t="s">
+        <v>1902</v>
+      </c>
+      <c r="D1240" s="44">
+        <f t="shared" si="72"/>
+        <v>670</v>
+      </c>
+      <c r="E1240" s="44">
+        <f t="shared" si="73"/>
+        <v>660</v>
+      </c>
+      <c r="F1240" s="66"/>
+      <c r="G1240" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1240" s="68"/>
+      <c r="I1240" s="119"/>
+      <c r="J1240" s="119"/>
+      <c r="K1240" s="96"/>
+      <c r="L1240" s="96"/>
+      <c r="M1240" s="80"/>
+      <c r="N1240" s="80"/>
+      <c r="O1240" s="69"/>
+      <c r="P1240" s="69"/>
+      <c r="Q1240" s="70">
+        <v>670</v>
+      </c>
+      <c r="R1240" s="70">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1241" s="1">
+        <v>1236</v>
+      </c>
+      <c r="B1241" s="66"/>
+      <c r="C1241" s="67" t="s">
+        <v>1903</v>
+      </c>
+      <c r="D1241" s="44">
+        <f t="shared" si="72"/>
+        <v>660</v>
+      </c>
+      <c r="E1241" s="44">
+        <f t="shared" si="73"/>
+        <v>650</v>
+      </c>
+      <c r="F1241" s="66"/>
+      <c r="G1241" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1241" s="68"/>
+      <c r="I1241" s="119"/>
+      <c r="J1241" s="119"/>
+      <c r="K1241" s="96"/>
+      <c r="L1241" s="96"/>
+      <c r="M1241" s="80"/>
+      <c r="N1241" s="80"/>
+      <c r="O1241" s="69"/>
+      <c r="P1241" s="69"/>
+      <c r="Q1241" s="70">
+        <v>660</v>
+      </c>
+      <c r="R1241" s="70">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1242" s="1">
+        <v>1237</v>
+      </c>
+      <c r="B1242" s="66"/>
+      <c r="C1242" s="67" t="s">
+        <v>1904</v>
+      </c>
+      <c r="D1242" s="44">
+        <f t="shared" si="72"/>
+        <v>635</v>
+      </c>
+      <c r="E1242" s="44">
+        <f t="shared" si="73"/>
+        <v>620</v>
+      </c>
+      <c r="F1242" s="66"/>
+      <c r="G1242" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1242" s="68"/>
+      <c r="I1242" s="119"/>
+      <c r="J1242" s="119"/>
+      <c r="K1242" s="96"/>
+      <c r="L1242" s="96"/>
+      <c r="M1242" s="80"/>
+      <c r="N1242" s="80"/>
+      <c r="O1242" s="69"/>
+      <c r="P1242" s="69"/>
+      <c r="Q1242" s="70">
+        <v>635</v>
+      </c>
+      <c r="R1242" s="70">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1243" s="1">
+        <v>1238</v>
+      </c>
+      <c r="B1243" s="66"/>
+      <c r="C1243" s="67" t="s">
+        <v>1905</v>
+      </c>
+      <c r="D1243" s="44">
+        <f t="shared" si="72"/>
+        <v>595</v>
+      </c>
+      <c r="E1243" s="44">
+        <f t="shared" si="73"/>
+        <v>590</v>
+      </c>
+      <c r="F1243" s="66"/>
+      <c r="G1243" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1243" s="68"/>
+      <c r="I1243" s="119"/>
+      <c r="J1243" s="119"/>
+      <c r="K1243" s="96"/>
+      <c r="L1243" s="96"/>
+      <c r="M1243" s="80"/>
+      <c r="N1243" s="80"/>
+      <c r="O1243" s="69"/>
+      <c r="P1243" s="69"/>
+      <c r="Q1243" s="70">
+        <v>595</v>
+      </c>
+      <c r="R1243" s="70">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1244" s="1">
+        <v>1239</v>
+      </c>
+      <c r="B1244" s="66"/>
+      <c r="C1244" s="67" t="s">
+        <v>1906</v>
+      </c>
+      <c r="D1244" s="44">
+        <f t="shared" si="72"/>
+        <v>590</v>
+      </c>
+      <c r="E1244" s="44">
+        <f t="shared" si="73"/>
+        <v>585</v>
+      </c>
+      <c r="F1244" s="66"/>
+      <c r="G1244" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1244" s="68"/>
+      <c r="I1244" s="119"/>
+      <c r="J1244" s="119"/>
+      <c r="K1244" s="96"/>
+      <c r="L1244" s="96"/>
+      <c r="M1244" s="80"/>
+      <c r="N1244" s="80"/>
+      <c r="O1244" s="69"/>
+      <c r="P1244" s="69"/>
+      <c r="Q1244" s="70">
+        <v>590</v>
+      </c>
+      <c r="R1244" s="70">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1245" s="1">
+        <v>1240</v>
+      </c>
+      <c r="B1245" s="66"/>
+      <c r="C1245" s="67" t="s">
+        <v>1907</v>
+      </c>
+      <c r="D1245" s="44">
+        <f t="shared" si="72"/>
+        <v>610</v>
+      </c>
+      <c r="E1245" s="44">
+        <f t="shared" si="73"/>
+        <v>600</v>
+      </c>
+      <c r="F1245" s="66"/>
+      <c r="G1245" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1245" s="68"/>
+      <c r="I1245" s="119"/>
+      <c r="J1245" s="119"/>
+      <c r="K1245" s="96"/>
+      <c r="L1245" s="96"/>
+      <c r="M1245" s="80"/>
+      <c r="N1245" s="80"/>
+      <c r="O1245" s="69"/>
+      <c r="P1245" s="69"/>
+      <c r="Q1245" s="70">
+        <v>610</v>
+      </c>
+      <c r="R1245" s="70">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1246" s="1">
+        <v>1241</v>
+      </c>
+      <c r="B1246" s="66"/>
+      <c r="C1246" s="67" t="s">
+        <v>1908</v>
+      </c>
+      <c r="D1246" s="44">
+        <f t="shared" si="72"/>
+        <v>605</v>
+      </c>
+      <c r="E1246" s="44">
+        <f t="shared" si="73"/>
+        <v>600</v>
+      </c>
+      <c r="F1246" s="66"/>
+      <c r="G1246" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1246" s="68"/>
+      <c r="I1246" s="119"/>
+      <c r="J1246" s="119"/>
+      <c r="K1246" s="96"/>
+      <c r="L1246" s="96"/>
+      <c r="M1246" s="80"/>
+      <c r="N1246" s="80"/>
+      <c r="O1246" s="69"/>
+      <c r="P1246" s="69"/>
+      <c r="Q1246" s="70">
+        <v>605</v>
+      </c>
+      <c r="R1246" s="70">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1247" s="1">
+        <v>1242</v>
+      </c>
+      <c r="B1247" s="66"/>
+      <c r="C1247" s="67" t="s">
+        <v>1909</v>
+      </c>
+      <c r="D1247" s="44">
+        <f t="shared" si="72"/>
+        <v>605</v>
+      </c>
+      <c r="E1247" s="44">
+        <f t="shared" si="73"/>
+        <v>600</v>
+      </c>
+      <c r="F1247" s="66"/>
+      <c r="G1247" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1247" s="68"/>
+      <c r="I1247" s="119"/>
+      <c r="J1247" s="119"/>
+      <c r="K1247" s="96"/>
+      <c r="L1247" s="96"/>
+      <c r="M1247" s="80"/>
+      <c r="N1247" s="80"/>
+      <c r="O1247" s="69"/>
+      <c r="P1247" s="69"/>
+      <c r="Q1247" s="70">
+        <v>605</v>
+      </c>
+      <c r="R1247" s="70">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1248" s="1">
+        <v>1243</v>
+      </c>
+      <c r="B1248" s="66"/>
+      <c r="C1248" s="67" t="s">
+        <v>1910</v>
+      </c>
+      <c r="D1248" s="44">
+        <f t="shared" si="72"/>
+        <v>600</v>
+      </c>
+      <c r="E1248" s="44">
+        <f t="shared" si="73"/>
+        <v>595</v>
+      </c>
+      <c r="F1248" s="66"/>
+      <c r="G1248" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1248" s="68"/>
+      <c r="I1248" s="119"/>
+      <c r="J1248" s="119"/>
+      <c r="K1248" s="96"/>
+      <c r="L1248" s="96"/>
+      <c r="M1248" s="80"/>
+      <c r="N1248" s="80"/>
+      <c r="O1248" s="69"/>
+      <c r="P1248" s="69"/>
+      <c r="Q1248" s="70">
+        <v>600</v>
+      </c>
+      <c r="R1248" s="70">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1249" s="1">
+        <v>1244</v>
+      </c>
+      <c r="B1249" s="66"/>
+      <c r="C1249" s="67" t="s">
+        <v>1911</v>
+      </c>
+      <c r="D1249" s="44">
+        <f t="shared" si="72"/>
+        <v>595</v>
+      </c>
+      <c r="E1249" s="44">
+        <f t="shared" si="73"/>
+        <v>590</v>
+      </c>
+      <c r="F1249" s="66"/>
+      <c r="G1249" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1249" s="68"/>
+      <c r="I1249" s="119"/>
+      <c r="J1249" s="119"/>
+      <c r="K1249" s="96"/>
+      <c r="L1249" s="96"/>
+      <c r="M1249" s="80"/>
+      <c r="N1249" s="80"/>
+      <c r="O1249" s="69"/>
+      <c r="P1249" s="69"/>
+      <c r="Q1249" s="70">
+        <v>595</v>
+      </c>
+      <c r="R1249" s="70">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1250" s="1">
+        <v>1245</v>
+      </c>
+      <c r="B1250" s="66"/>
+      <c r="C1250" s="67" t="s">
+        <v>1912</v>
+      </c>
+      <c r="D1250" s="44">
+        <f t="shared" si="72"/>
+        <v>590</v>
+      </c>
+      <c r="E1250" s="44">
+        <f t="shared" si="73"/>
+        <v>585</v>
+      </c>
+      <c r="F1250" s="66"/>
+      <c r="G1250" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1250" s="68"/>
+      <c r="I1250" s="119"/>
+      <c r="J1250" s="119"/>
+      <c r="K1250" s="96"/>
+      <c r="L1250" s="96"/>
+      <c r="M1250" s="80"/>
+      <c r="N1250" s="80"/>
+      <c r="O1250" s="69"/>
+      <c r="P1250" s="69"/>
+      <c r="Q1250" s="70">
+        <v>590</v>
+      </c>
+      <c r="R1250" s="70">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1251" s="1">
+        <v>1246</v>
+      </c>
+      <c r="B1251" s="66"/>
+      <c r="C1251" s="67" t="s">
+        <v>1913</v>
+      </c>
+      <c r="D1251" s="44">
+        <f t="shared" si="72"/>
+        <v>685</v>
+      </c>
+      <c r="E1251" s="44">
+        <f t="shared" si="73"/>
+        <v>670</v>
+      </c>
+      <c r="F1251" s="66"/>
+      <c r="G1251" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1251" s="68"/>
+      <c r="I1251" s="119"/>
+      <c r="J1251" s="119"/>
+      <c r="K1251" s="96"/>
+      <c r="L1251" s="96"/>
+      <c r="M1251" s="80"/>
+      <c r="N1251" s="80"/>
+      <c r="O1251" s="69"/>
+      <c r="P1251" s="69"/>
+      <c r="Q1251" s="70">
+        <v>685</v>
+      </c>
+      <c r="R1251" s="70">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1252" s="1">
+        <v>1247</v>
+      </c>
+      <c r="B1252" s="66"/>
+      <c r="C1252" s="67" t="s">
+        <v>1914</v>
+      </c>
+      <c r="D1252" s="44">
+        <f t="shared" si="72"/>
+        <v>640</v>
+      </c>
+      <c r="E1252" s="44">
+        <f t="shared" si="73"/>
+        <v>630</v>
+      </c>
+      <c r="F1252" s="66"/>
+      <c r="G1252" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1252" s="68"/>
+      <c r="I1252" s="119"/>
+      <c r="J1252" s="119"/>
+      <c r="K1252" s="96"/>
+      <c r="L1252" s="96"/>
+      <c r="M1252" s="80"/>
+      <c r="N1252" s="80"/>
+      <c r="O1252" s="69"/>
+      <c r="P1252" s="69"/>
+      <c r="Q1252" s="70">
+        <v>640</v>
+      </c>
+      <c r="R1252" s="70">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1253" s="1">
+        <v>1248</v>
+      </c>
+      <c r="B1253" s="66"/>
+      <c r="C1253" s="67" t="s">
+        <v>1915</v>
+      </c>
+      <c r="D1253" s="44">
+        <f t="shared" si="72"/>
+        <v>640</v>
+      </c>
+      <c r="E1253" s="44">
+        <f t="shared" si="73"/>
+        <v>630</v>
+      </c>
+      <c r="F1253" s="66"/>
+      <c r="G1253" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1253" s="68"/>
+      <c r="I1253" s="119"/>
+      <c r="J1253" s="119"/>
+      <c r="K1253" s="96"/>
+      <c r="L1253" s="96"/>
+      <c r="M1253" s="80"/>
+      <c r="N1253" s="80"/>
+      <c r="O1253" s="69"/>
+      <c r="P1253" s="69"/>
+      <c r="Q1253" s="70">
+        <v>640</v>
+      </c>
+      <c r="R1253" s="70">
+        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -54167,7 +54941,7 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="Q4:R4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1238:C1048576 C1:C3">
+  <conditionalFormatting sqref="C1254:C1048576 C1:C3">
     <cfRule type="duplicateValues" dxfId="10" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C5">
@@ -54191,7 +54965,7 @@
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1059:C1149 C1151:C1237">
+  <conditionalFormatting sqref="C1059:C1149 C1151:C1253">
     <cfRule type="duplicateValues" dxfId="2" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C160 C987:C1149 C965:C985 C888:C963 C792:C886 C775:C790 C745:C773 C741:C743 C707:C739 C497:C705 C474:C495 C444:C472 C388:C442 C359:C386 C324:C357 C312:C322 C296:C310 C288:C294 C282:C286 C276:C280 C252:C274 C247:C250 C224:C245 C197:C222 C162:C195 C1151:C1048576">

</xml_diff>

<commit_message>
chore: update score and node 18
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEAC20E-1370-B94B-8841-313E414810F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A761DCC-B647-B048-B214-0F212B02CFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7949,8 +7949,8 @@
   <dimension ref="A1:U1254"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A1232" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S1254" sqref="S1254"/>
+      <pane ySplit="5" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I166" sqref="I166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14264,7 +14264,7 @@
       </c>
       <c r="D165" s="44">
         <f t="shared" si="14"/>
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="E165" s="44">
         <f t="shared" si="15"/>
@@ -14275,7 +14275,9 @@
         <v>1</v>
       </c>
       <c r="H165" s="14"/>
-      <c r="I165" s="112"/>
+      <c r="I165" s="112">
+        <v>-5</v>
+      </c>
       <c r="J165" s="112"/>
       <c r="K165" s="96">
         <v>-5</v>

</xml_diff>

<commit_message>
chore: update nhu van phuc
</commit_message>
<xml_diff>
--- a/scripts/data.xlsx
+++ b/scripts/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duongital/Programming/node/dflyapp/tennis-btn/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A761DCC-B647-B048-B214-0F212B02CFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3156FC-9EAE-EC4E-9FF5-051AE5D53897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="760" windowWidth="29080" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="1917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="1918">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -5822,6 +5822,9 @@
   </si>
   <si>
     <t>Nghị Nho CT</t>
+  </si>
+  <si>
+    <t>Tý sản</t>
   </si>
 </sst>
 </file>
@@ -7946,11 +7949,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U1254"/>
+  <dimension ref="A1:U1255"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I166" sqref="I166"/>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A1237" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1254" sqref="G1254:G1255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -54950,11 +54953,11 @@
         <v>1916</v>
       </c>
       <c r="D1254" s="44">
-        <f t="shared" ref="D1254" si="74">Q1254+O1254+M1254+K1254+I1254</f>
+        <f t="shared" ref="D1254:D1255" si="74">Q1254+O1254+M1254+K1254+I1254</f>
         <v>620</v>
       </c>
       <c r="E1254" s="44">
-        <f t="shared" ref="E1254" si="75">P1254+R1254+N1254+L1254+J1254</f>
+        <f t="shared" ref="E1254:E1255" si="75">P1254+R1254+N1254+L1254+J1254</f>
         <v>610</v>
       </c>
       <c r="F1254" s="66"/>
@@ -54977,6 +54980,42 @@
         <v>610</v>
       </c>
     </row>
+    <row r="1255" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1255" s="1">
+        <v>1250</v>
+      </c>
+      <c r="B1255" s="66"/>
+      <c r="C1255" s="67" t="s">
+        <v>1917</v>
+      </c>
+      <c r="D1255" s="44">
+        <f t="shared" si="74"/>
+        <v>675</v>
+      </c>
+      <c r="E1255" s="44">
+        <f t="shared" si="75"/>
+        <v>670</v>
+      </c>
+      <c r="F1255" s="66"/>
+      <c r="G1255" s="47">
+        <v>1</v>
+      </c>
+      <c r="H1255" s="68"/>
+      <c r="I1255" s="119"/>
+      <c r="J1255" s="119"/>
+      <c r="K1255" s="96"/>
+      <c r="L1255" s="96"/>
+      <c r="M1255" s="80"/>
+      <c r="N1255" s="80"/>
+      <c r="O1255" s="69"/>
+      <c r="P1255" s="69"/>
+      <c r="Q1255" s="70">
+        <v>675</v>
+      </c>
+      <c r="R1255" s="70">
+        <v>670</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0"/>
   <autoFilter ref="A4:J1230" xr:uid="{00000000-0001-0000-0100-000000000000}">
@@ -54988,7 +55027,7 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="Q4:R4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1255:C1048576 C1:C3">
+  <conditionalFormatting sqref="C1256:C1048576 C1:C3">
     <cfRule type="duplicateValues" dxfId="10" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C5">
@@ -55012,7 +55051,7 @@
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1059:C1149 C1151:C1254">
+  <conditionalFormatting sqref="C1059:C1149 C1151:C1255">
     <cfRule type="duplicateValues" dxfId="2" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C160 C987:C1149 C965:C985 C888:C963 C792:C886 C775:C790 C745:C773 C741:C743 C707:C739 C497:C705 C474:C495 C444:C472 C388:C442 C359:C386 C324:C357 C312:C322 C296:C310 C288:C294 C282:C286 C276:C280 C252:C274 C247:C250 C224:C245 C197:C222 C162:C195 C1151:C1048576">
@@ -55035,9 +55074,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J1:J1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -58507,7 +58546,7 @@
       </c>
       <c r="D92" s="84">
         <f t="shared" si="4"/>
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="E92" s="84">
         <f t="shared" si="5"/>
@@ -58519,7 +58558,9 @@
       <c r="G92" s="85">
         <v>1</v>
       </c>
-      <c r="H92" s="123"/>
+      <c r="H92" s="123">
+        <v>-5</v>
+      </c>
       <c r="I92" s="123"/>
       <c r="J92" s="47"/>
       <c r="K92" s="86"/>

</xml_diff>